<commit_message>
Updated Gantt and Caravel stuff
</commit_message>
<xml_diff>
--- a/Docs/Team_Gantt_Chart.xlsx
+++ b/Docs/Team_Gantt_Chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Brandon Foss\Documents\GitHub\6_Angry_Devs\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5342F63-71F4-481E-905D-F94F820F02C7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EA66186-94BA-4E59-BB82-C804275FE8C4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="12030" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="90">
   <si>
     <t>testing</t>
   </si>
@@ -188,9 +188,6 @@
     <t>User Customizable Input</t>
   </si>
   <si>
-    <t>Implementing menu</t>
-  </si>
-  <si>
     <t>Totals</t>
   </si>
   <si>
@@ -236,9 +233,6 @@
     <t>terrain effects</t>
   </si>
   <si>
-    <t>demo/AI</t>
-  </si>
-  <si>
     <t>Writing RFP - 2.0</t>
   </si>
   <si>
@@ -282,6 +276,33 @@
   </si>
   <si>
     <t>Feb. 11</t>
+  </si>
+  <si>
+    <t>create caravel physics</t>
+  </si>
+  <si>
+    <t>level creation</t>
+  </si>
+  <si>
+    <t>perk system</t>
+  </si>
+  <si>
+    <t>pause menu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">end screen </t>
+  </si>
+  <si>
+    <t>demo/stress test</t>
+  </si>
+  <si>
+    <t>Gantt Chart Demo Prep</t>
+  </si>
+  <si>
+    <t>Mar. 25</t>
+  </si>
+  <si>
+    <t>barrel physics</t>
   </si>
 </sst>
 </file>
@@ -384,7 +405,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="28">
+  <borders count="30">
     <border>
       <left/>
       <right/>
@@ -739,11 +760,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="109">
+  <cellXfs count="111">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -863,7 +904,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -873,6 +913,9 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1190,7 +1233,7 @@
   <dimension ref="B1:Q10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+      <selection activeCell="P25" sqref="P25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1214,27 +1257,27 @@
   <sheetData>
     <row r="1" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="C2" s="106" t="s">
+      <c r="C2" s="105" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="107"/>
-      <c r="E2" s="108"/>
+      <c r="D2" s="106"/>
+      <c r="E2" s="107"/>
       <c r="F2" s="6"/>
-      <c r="G2" s="106" t="s">
+      <c r="G2" s="105" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="107"/>
-      <c r="I2" s="108"/>
-      <c r="K2" s="106" t="s">
+      <c r="H2" s="106"/>
+      <c r="I2" s="107"/>
+      <c r="K2" s="105" t="s">
         <v>7</v>
       </c>
-      <c r="L2" s="107"/>
-      <c r="M2" s="108"/>
-      <c r="O2" s="106" t="s">
+      <c r="L2" s="106"/>
+      <c r="M2" s="107"/>
+      <c r="O2" s="105" t="s">
         <v>26</v>
       </c>
-      <c r="P2" s="107"/>
-      <c r="Q2" s="108"/>
+      <c r="P2" s="106"/>
+      <c r="Q2" s="107"/>
     </row>
     <row r="3" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C3" s="7" t="s">
@@ -1281,39 +1324,39 @@
       </c>
       <c r="C4" s="20">
         <f>(G4+K4 +O4)</f>
-        <v>6000</v>
+        <v>7000</v>
       </c>
       <c r="D4" s="21">
         <f t="shared" ref="D4:D7" si="0">(H4+L4 +P4)</f>
-        <v>4450</v>
+        <v>5750</v>
       </c>
       <c r="E4" s="22">
         <f>(C4-D4)</f>
-        <v>1550</v>
+        <v>1250</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="14">
         <f>(Gantt!$B10)*100</f>
-        <v>2700</v>
+        <v>3700</v>
       </c>
       <c r="H4" s="15">
         <f>(Gantt!$C10)*100</f>
-        <v>2000</v>
+        <v>3100</v>
       </c>
       <c r="I4" s="16">
         <f>(G4-H4)</f>
-        <v>700</v>
+        <v>600</v>
       </c>
       <c r="K4" s="20">
         <v>2000</v>
       </c>
       <c r="L4" s="21">
         <f>Meetings!B4*100</f>
-        <v>1150</v>
+        <v>1350</v>
       </c>
       <c r="M4" s="22">
         <f>(K4-L4)</f>
-        <v>850</v>
+        <v>650</v>
       </c>
       <c r="O4" s="47">
         <f>(SA!C7)*100</f>
@@ -1334,39 +1377,39 @@
       </c>
       <c r="C5" s="14">
         <f t="shared" ref="C5:C7" si="1">(G5+K5 +O5)</f>
-        <v>11500</v>
+        <v>13000</v>
       </c>
       <c r="D5" s="15">
         <f t="shared" si="0"/>
-        <v>6550</v>
+        <v>8150</v>
       </c>
       <c r="E5" s="16">
         <f t="shared" ref="E5:E7" si="2">(C5-D5)</f>
-        <v>4950</v>
+        <v>4850</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="14">
         <f>(Gantt!$B20)*100</f>
-        <v>8300</v>
+        <v>9800</v>
       </c>
       <c r="H5" s="15">
         <f>(Gantt!$C20)*100</f>
-        <v>4200</v>
+        <v>5600</v>
       </c>
       <c r="I5" s="16">
         <f t="shared" ref="I5:I7" si="3">(G5-H5)</f>
-        <v>4100</v>
+        <v>4200</v>
       </c>
       <c r="K5" s="47">
         <v>2000</v>
       </c>
       <c r="L5" s="15">
         <f>Meetings!B5*100</f>
-        <v>1150</v>
+        <v>1350</v>
       </c>
       <c r="M5" s="16">
         <f t="shared" ref="M5:M7" si="4">(K5-L5)</f>
-        <v>850</v>
+        <v>650</v>
       </c>
       <c r="O5" s="44">
         <f>(SA!C12)*100</f>
@@ -1391,11 +1434,11 @@
       </c>
       <c r="D6" s="15">
         <f t="shared" si="0"/>
-        <v>3450</v>
+        <v>4250</v>
       </c>
       <c r="E6" s="16">
         <f t="shared" si="2"/>
-        <v>2750</v>
+        <v>1950</v>
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="14">
@@ -1404,22 +1447,22 @@
       </c>
       <c r="H6" s="15">
         <f>(Gantt!$C28)*100</f>
-        <v>1400</v>
+        <v>2000</v>
       </c>
       <c r="I6" s="16">
         <f t="shared" si="3"/>
-        <v>1600</v>
+        <v>1000</v>
       </c>
       <c r="K6" s="47">
         <v>2000</v>
       </c>
       <c r="L6" s="15">
         <f>Meetings!B6*100</f>
-        <v>950</v>
+        <v>1150</v>
       </c>
       <c r="M6" s="16">
         <f t="shared" si="4"/>
-        <v>1050</v>
+        <v>850</v>
       </c>
       <c r="N6" s="42"/>
       <c r="O6" s="45">
@@ -1441,24 +1484,24 @@
       </c>
       <c r="C7" s="45">
         <f t="shared" si="1"/>
-        <v>5400</v>
+        <v>3800</v>
       </c>
       <c r="D7" s="45">
         <f t="shared" si="0"/>
-        <v>4100</v>
+        <v>2700</v>
       </c>
       <c r="E7" s="46">
         <f t="shared" si="2"/>
-        <v>1300</v>
+        <v>1100</v>
       </c>
       <c r="F7" s="3"/>
       <c r="G7" s="14">
         <f>(Gantt!$B36)*100</f>
-        <v>2200</v>
+        <v>600</v>
       </c>
       <c r="H7" s="15">
         <f>(Gantt!$C36)*100</f>
-        <v>2000</v>
+        <v>400</v>
       </c>
       <c r="I7" s="16">
         <f t="shared" si="3"/>
@@ -1469,11 +1512,11 @@
       </c>
       <c r="L7" s="15">
         <f>Meetings!B7*100</f>
-        <v>1000</v>
+        <v>1200</v>
       </c>
       <c r="M7" s="16">
         <f t="shared" si="4"/>
-        <v>1000</v>
+        <v>800</v>
       </c>
       <c r="N7" s="42"/>
       <c r="O7" s="56">
@@ -1495,28 +1538,28 @@
       </c>
       <c r="C8" s="45">
         <f t="shared" ref="C8:C9" si="6">(G8+K8 +O8)</f>
-        <v>7800</v>
+        <v>4700</v>
       </c>
       <c r="D8" s="45">
         <f t="shared" ref="D8:D9" si="7">(H8+L8 +P8)</f>
-        <v>3350</v>
+        <v>2450</v>
       </c>
       <c r="E8" s="46">
         <f t="shared" ref="E8:E9" si="8">(C8-D8)</f>
-        <v>4450</v>
+        <v>2250</v>
       </c>
       <c r="F8" s="3"/>
       <c r="G8" s="14">
         <f>(Gantt!$B44)*100</f>
-        <v>4600</v>
+        <v>1500</v>
       </c>
       <c r="H8" s="15">
         <f>(Gantt!$C44)*100</f>
-        <v>1200</v>
+        <v>300</v>
       </c>
       <c r="I8" s="16">
         <f t="shared" ref="I8:I9" si="9">(G8-H8)</f>
-        <v>3400</v>
+        <v>1200</v>
       </c>
       <c r="K8" s="47">
         <v>2000</v>
@@ -1549,27 +1592,27 @@
       </c>
       <c r="C9" s="40">
         <f t="shared" si="6"/>
-        <v>4400</v>
+        <v>3700</v>
       </c>
       <c r="D9" s="41">
         <f t="shared" si="7"/>
-        <v>1350</v>
+        <v>1150</v>
       </c>
       <c r="E9" s="27">
         <f t="shared" si="8"/>
-        <v>3050</v>
+        <v>2550</v>
       </c>
       <c r="G9" s="14">
         <f>(Gantt!$B52)*100</f>
-        <v>1200</v>
+        <v>500</v>
       </c>
       <c r="H9" s="15">
         <f>(Gantt!$C52)*100</f>
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="I9" s="16">
         <f t="shared" si="9"/>
-        <v>800</v>
+        <v>300</v>
       </c>
       <c r="K9" s="47">
         <v>2000</v>
@@ -1601,27 +1644,27 @@
       </c>
       <c r="C10" s="24">
         <f>SUM(C4:C9)</f>
-        <v>41300</v>
+        <v>38400</v>
       </c>
       <c r="D10" s="25">
         <f>SUM(D4:D9)</f>
-        <v>23250</v>
+        <v>24450</v>
       </c>
       <c r="E10" s="26">
         <f>SUM(E4:E9)</f>
-        <v>18050</v>
+        <v>13950</v>
       </c>
       <c r="G10" s="17">
         <f>SUM(G4:G9)</f>
-        <v>22000</v>
+        <v>19100</v>
       </c>
       <c r="H10" s="18">
         <f>SUM(H4:H9)</f>
-        <v>11200</v>
+        <v>11600</v>
       </c>
       <c r="I10" s="19">
         <f>SUM(I4:I9)</f>
-        <v>10800</v>
+        <v>7500</v>
       </c>
       <c r="K10" s="17">
         <f>SUM(K4:K9)</f>
@@ -1629,11 +1672,11 @@
       </c>
       <c r="L10" s="18">
         <f>SUM(L4:L9)</f>
-        <v>5750</v>
+        <v>6550</v>
       </c>
       <c r="M10" s="19">
         <f>SUM(M4:M9)</f>
-        <v>6250</v>
+        <v>5450</v>
       </c>
       <c r="O10" s="24">
         <f>SUM(O4:O9)</f>
@@ -1662,10 +1705,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AF66"/>
+  <dimension ref="A1:AN66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H51" sqref="H51"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="J36" sqref="J36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1676,15 +1719,15 @@
     <col min="6" max="6" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" t="s">
         <v>55</v>
       </c>
-      <c r="C1" t="s">
-        <v>56</v>
-      </c>
       <c r="D1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" t="s">
@@ -1699,14 +1742,14 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A2" s="87" t="s">
         <v>27</v>
       </c>
       <c r="B2" s="88"/>
       <c r="C2" s="88"/>
       <c r="D2" s="89" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E2" s="90">
         <v>3</v>
@@ -1789,8 +1832,35 @@
       <c r="AE2" s="91">
         <v>81</v>
       </c>
-    </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AF2" s="90">
+        <v>84</v>
+      </c>
+      <c r="AG2" s="90">
+        <v>87</v>
+      </c>
+      <c r="AH2" s="90">
+        <v>90</v>
+      </c>
+      <c r="AI2" s="90">
+        <v>93</v>
+      </c>
+      <c r="AJ2" s="90">
+        <v>96</v>
+      </c>
+      <c r="AK2" s="90">
+        <v>98</v>
+      </c>
+      <c r="AL2" s="90">
+        <v>101</v>
+      </c>
+      <c r="AM2" s="90">
+        <v>104</v>
+      </c>
+      <c r="AN2" s="91">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="3" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A3" s="92" t="s">
         <v>42</v>
       </c>
@@ -1827,17 +1897,18 @@
       <c r="AB3" s="51"/>
       <c r="AC3" s="51"/>
       <c r="AD3" s="51"/>
-      <c r="AE3" s="52"/>
-    </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AE3" s="109"/>
+      <c r="AN3" s="110"/>
+    </row>
+    <row r="4" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A4" s="92" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B4" s="69">
         <v>6</v>
       </c>
       <c r="C4" s="69">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D4" s="51"/>
       <c r="E4" s="51"/>
@@ -1866,24 +1937,25 @@
       <c r="AB4" s="51"/>
       <c r="AC4" s="51"/>
       <c r="AD4" s="51"/>
-      <c r="AE4" s="52"/>
-    </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AE4" s="51"/>
+      <c r="AN4" s="52"/>
+    </row>
+    <row r="5" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A5" s="92" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B5" s="69">
         <v>3</v>
       </c>
       <c r="C5" s="69">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D5" s="51"/>
       <c r="E5" s="51"/>
       <c r="F5" s="51"/>
       <c r="G5" s="51"/>
       <c r="H5" s="93"/>
-      <c r="I5" s="51"/>
+      <c r="I5" s="93"/>
       <c r="J5" s="51"/>
       <c r="K5" s="51"/>
       <c r="L5" s="51"/>
@@ -1905,28 +1977,29 @@
       <c r="AB5" s="51"/>
       <c r="AC5" s="51"/>
       <c r="AD5" s="51"/>
-      <c r="AE5" s="52"/>
-    </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AE5" s="51"/>
+      <c r="AN5" s="52"/>
+    </row>
+    <row r="6" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A6" s="92" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B6" s="69">
         <v>12</v>
       </c>
       <c r="C6" s="69">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D6" s="51"/>
       <c r="E6" s="51"/>
       <c r="F6" s="51"/>
       <c r="G6" s="51"/>
       <c r="H6" s="51"/>
-      <c r="I6" s="93"/>
-      <c r="J6" s="104"/>
-      <c r="K6" s="94"/>
-      <c r="L6" s="94"/>
-      <c r="M6" s="51"/>
+      <c r="I6" s="51"/>
+      <c r="J6" s="93"/>
+      <c r="K6" s="93"/>
+      <c r="L6" s="104"/>
+      <c r="M6" s="94"/>
       <c r="N6" s="51"/>
       <c r="O6" s="51"/>
       <c r="P6" s="51"/>
@@ -1944,17 +2017,18 @@
       <c r="AB6" s="51"/>
       <c r="AC6" s="51"/>
       <c r="AD6" s="51"/>
-      <c r="AE6" s="52"/>
-    </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AE6" s="51"/>
+      <c r="AN6" s="52"/>
+    </row>
+    <row r="7" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A7" s="92" t="s">
-        <v>35</v>
+        <v>81</v>
       </c>
       <c r="B7" s="69">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C7" s="69">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D7" s="51"/>
       <c r="E7" s="51"/>
@@ -1966,7 +2040,7 @@
       <c r="K7" s="51"/>
       <c r="L7" s="51"/>
       <c r="M7" s="51"/>
-      <c r="N7" s="51"/>
+      <c r="N7" s="93"/>
       <c r="O7" s="51"/>
       <c r="P7" s="51"/>
       <c r="Q7" s="51"/>
@@ -1983,17 +2057,18 @@
       <c r="AB7" s="51"/>
       <c r="AC7" s="51"/>
       <c r="AD7" s="51"/>
-      <c r="AE7" s="52"/>
-    </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AE7" s="51"/>
+      <c r="AN7" s="52"/>
+    </row>
+    <row r="8" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A8" s="92" t="s">
-        <v>35</v>
+        <v>82</v>
       </c>
       <c r="B8" s="69">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C8" s="69">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D8" s="51"/>
       <c r="E8" s="51"/>
@@ -2006,9 +2081,9 @@
       <c r="L8" s="51"/>
       <c r="M8" s="51"/>
       <c r="N8" s="51"/>
-      <c r="O8" s="51"/>
-      <c r="P8" s="51"/>
-      <c r="Q8" s="51"/>
+      <c r="O8" s="93"/>
+      <c r="P8" s="93"/>
+      <c r="Q8" s="104"/>
       <c r="R8" s="51"/>
       <c r="S8" s="51"/>
       <c r="T8" s="51"/>
@@ -2022,9 +2097,10 @@
       <c r="AB8" s="51"/>
       <c r="AC8" s="51"/>
       <c r="AD8" s="51"/>
-      <c r="AE8" s="52"/>
-    </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AE8" s="51"/>
+      <c r="AN8" s="52"/>
+    </row>
+    <row r="9" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A9" s="92" t="s">
         <v>0</v>
       </c>
@@ -2032,7 +2108,7 @@
         <v>3</v>
       </c>
       <c r="C9" s="69">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D9" s="51"/>
       <c r="E9" s="51"/>
@@ -2043,12 +2119,12 @@
       <c r="J9" s="51"/>
       <c r="K9" s="59"/>
       <c r="L9" s="59"/>
-      <c r="M9" s="93"/>
+      <c r="M9" s="59"/>
       <c r="N9" s="51"/>
       <c r="O9" s="51"/>
       <c r="P9" s="51"/>
       <c r="Q9" s="51"/>
-      <c r="R9" s="51"/>
+      <c r="R9" s="93"/>
       <c r="S9" s="51"/>
       <c r="T9" s="51"/>
       <c r="U9" s="51"/>
@@ -2061,19 +2137,20 @@
       <c r="AB9" s="51"/>
       <c r="AC9" s="51"/>
       <c r="AD9" s="51"/>
-      <c r="AE9" s="52"/>
-    </row>
-    <row r="10" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AE9" s="51"/>
+      <c r="AN9" s="52"/>
+    </row>
+    <row r="10" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="72" t="s">
         <v>1</v>
       </c>
       <c r="B10" s="95">
         <f>SUM(B3:B9)</f>
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="C10" s="95">
         <f>SUM(C3:C9)</f>
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="D10" s="96"/>
       <c r="E10" s="96"/>
@@ -2102,9 +2179,18 @@
       <c r="AB10" s="96"/>
       <c r="AC10" s="96"/>
       <c r="AD10" s="96"/>
-      <c r="AE10" s="97"/>
-    </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AE10" s="96"/>
+      <c r="AF10" s="96"/>
+      <c r="AG10" s="96"/>
+      <c r="AH10" s="96"/>
+      <c r="AI10" s="96"/>
+      <c r="AJ10" s="96"/>
+      <c r="AK10" s="96"/>
+      <c r="AL10" s="96"/>
+      <c r="AM10" s="96"/>
+      <c r="AN10" s="97"/>
+    </row>
+    <row r="11" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A11" s="98" t="s">
         <v>28</v>
       </c>
@@ -2137,9 +2223,10 @@
       <c r="AB11" s="60"/>
       <c r="AC11" s="60"/>
       <c r="AD11" s="60"/>
-      <c r="AE11" s="61"/>
-    </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AE11" s="60"/>
+      <c r="AN11" s="52"/>
+    </row>
+    <row r="12" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A12" s="92" t="s">
         <v>40</v>
       </c>
@@ -2176,17 +2263,18 @@
       <c r="AB12" s="51"/>
       <c r="AC12" s="51"/>
       <c r="AD12" s="51"/>
-      <c r="AE12" s="52"/>
-    </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AE12" s="51"/>
+      <c r="AN12" s="52"/>
+    </row>
+    <row r="13" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A13" s="92" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B13" s="69">
         <v>5</v>
       </c>
       <c r="C13" s="69">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="D13" s="51"/>
       <c r="E13" s="51"/>
@@ -2194,7 +2282,7 @@
       <c r="G13" s="93"/>
       <c r="H13" s="93"/>
       <c r="I13" s="93"/>
-      <c r="J13" s="51"/>
+      <c r="J13" s="93"/>
       <c r="K13" s="51"/>
       <c r="L13" s="51"/>
       <c r="M13" s="51"/>
@@ -2215,17 +2303,18 @@
       <c r="AB13" s="51"/>
       <c r="AC13" s="51"/>
       <c r="AD13" s="51"/>
-      <c r="AE13" s="52"/>
-    </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AE13" s="51"/>
+      <c r="AN13" s="52"/>
+    </row>
+    <row r="14" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A14" s="92" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B14" s="69">
         <v>5</v>
       </c>
       <c r="C14" s="69">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D14" s="51"/>
       <c r="E14" s="51"/>
@@ -2233,11 +2322,11 @@
       <c r="G14" s="51"/>
       <c r="H14" s="59"/>
       <c r="I14" s="59"/>
-      <c r="J14" s="93"/>
+      <c r="J14" s="59"/>
       <c r="K14" s="93"/>
       <c r="L14" s="93"/>
-      <c r="M14" s="51"/>
-      <c r="N14" s="51"/>
+      <c r="M14" s="93"/>
+      <c r="N14" s="93"/>
       <c r="O14" s="51"/>
       <c r="P14" s="51"/>
       <c r="Q14" s="51"/>
@@ -2254,17 +2343,18 @@
       <c r="AB14" s="51"/>
       <c r="AC14" s="51"/>
       <c r="AD14" s="51"/>
-      <c r="AE14" s="52"/>
-    </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AE14" s="51"/>
+      <c r="AN14" s="52"/>
+    </row>
+    <row r="15" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A15" s="92" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B15" s="69">
         <v>30</v>
       </c>
       <c r="C15" s="69">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D15" s="51"/>
       <c r="E15" s="51"/>
@@ -2275,29 +2365,30 @@
       <c r="J15" s="51"/>
       <c r="K15" s="51"/>
       <c r="L15" s="51"/>
-      <c r="M15" s="93"/>
-      <c r="N15" s="93"/>
+      <c r="M15" s="51"/>
+      <c r="N15" s="51"/>
       <c r="O15" s="93"/>
       <c r="P15" s="93"/>
-      <c r="Q15" s="104"/>
-      <c r="R15" s="94"/>
-      <c r="S15" s="94"/>
-      <c r="T15" s="51"/>
-      <c r="U15" s="51"/>
-      <c r="V15" s="51"/>
-      <c r="W15" s="51"/>
-      <c r="X15" s="51"/>
+      <c r="Q15" s="93"/>
+      <c r="R15" s="93"/>
+      <c r="S15" s="93"/>
+      <c r="T15" s="104"/>
+      <c r="U15" s="94"/>
+      <c r="V15" s="94"/>
+      <c r="W15" s="94"/>
+      <c r="X15" s="94"/>
       <c r="Y15" s="51"/>
       <c r="Z15" s="51"/>
       <c r="AA15" s="51"/>
       <c r="AB15" s="51"/>
       <c r="AC15" s="51"/>
       <c r="AD15" s="51"/>
-      <c r="AE15" s="52"/>
-    </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AE15" s="51"/>
+      <c r="AN15" s="52"/>
+    </row>
+    <row r="16" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A16" s="92" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B16" s="69">
         <v>20</v>
@@ -2321,28 +2412,29 @@
       <c r="Q16" s="51"/>
       <c r="R16" s="51"/>
       <c r="S16" s="51"/>
-      <c r="T16" s="93"/>
-      <c r="U16" s="93"/>
-      <c r="V16" s="94"/>
-      <c r="W16" s="94"/>
-      <c r="X16" s="94"/>
-      <c r="Y16" s="94"/>
-      <c r="Z16" s="51"/>
-      <c r="AA16" s="51"/>
-      <c r="AB16" s="51"/>
-      <c r="AC16" s="51"/>
-      <c r="AD16" s="51"/>
-      <c r="AE16" s="52"/>
-    </row>
-    <row r="17" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="T16" s="51"/>
+      <c r="U16" s="51"/>
+      <c r="V16" s="51"/>
+      <c r="W16" s="51"/>
+      <c r="X16" s="51"/>
+      <c r="Y16" s="93"/>
+      <c r="Z16" s="104"/>
+      <c r="AA16" s="94"/>
+      <c r="AB16" s="94"/>
+      <c r="AC16" s="94"/>
+      <c r="AD16" s="94"/>
+      <c r="AE16" s="94"/>
+      <c r="AN16" s="52"/>
+    </row>
+    <row r="17" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A17" s="92" t="s">
-        <v>35</v>
+        <v>83</v>
       </c>
       <c r="B17" s="69">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="C17" s="69">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D17" s="51"/>
       <c r="E17" s="51"/>
@@ -2371,10 +2463,15 @@
       <c r="AB17" s="51"/>
       <c r="AC17" s="51"/>
       <c r="AD17" s="51"/>
-      <c r="AE17" s="52"/>
-      <c r="AF17" s="3"/>
-    </row>
-    <row r="18" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AE17" s="51"/>
+      <c r="AF17" s="2"/>
+      <c r="AG17" s="4"/>
+      <c r="AH17" s="4"/>
+      <c r="AI17" s="4"/>
+      <c r="AJ17" s="4"/>
+      <c r="AN17" s="52"/>
+    </row>
+    <row r="18" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A18" s="92" t="s">
         <v>35</v>
       </c>
@@ -2411,9 +2508,10 @@
       <c r="AB18" s="51"/>
       <c r="AC18" s="51"/>
       <c r="AD18" s="51"/>
-      <c r="AE18" s="52"/>
-    </row>
-    <row r="19" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AE18" s="51"/>
+      <c r="AN18" s="52"/>
+    </row>
+    <row r="19" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A19" s="92" t="s">
         <v>0</v>
       </c>
@@ -2445,24 +2543,28 @@
       <c r="W19" s="51"/>
       <c r="X19" s="51"/>
       <c r="Y19" s="51"/>
-      <c r="Z19" s="93"/>
-      <c r="AA19" s="94"/>
-      <c r="AB19" s="94"/>
-      <c r="AC19" s="94"/>
-      <c r="AD19" s="94"/>
-      <c r="AE19" s="99"/>
-    </row>
-    <row r="20" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z19" s="51"/>
+      <c r="AA19" s="51"/>
+      <c r="AB19" s="51"/>
+      <c r="AC19" s="51"/>
+      <c r="AD19" s="51"/>
+      <c r="AE19" s="51"/>
+      <c r="AK19" s="108"/>
+      <c r="AL19" s="4"/>
+      <c r="AM19" s="4"/>
+      <c r="AN19" s="99"/>
+    </row>
+    <row r="20" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="72" t="s">
         <v>1</v>
       </c>
       <c r="B20" s="95">
         <f>SUM(B12:B19)</f>
-        <v>83</v>
+        <v>98</v>
       </c>
       <c r="C20" s="95">
         <f>SUM(C12:C19)</f>
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="D20" s="96"/>
       <c r="E20" s="96"/>
@@ -2492,8 +2594,17 @@
       <c r="AC20" s="96"/>
       <c r="AD20" s="96"/>
       <c r="AE20" s="96"/>
-    </row>
-    <row r="21" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AF20" s="96"/>
+      <c r="AG20" s="96"/>
+      <c r="AH20" s="96"/>
+      <c r="AI20" s="96"/>
+      <c r="AJ20" s="96"/>
+      <c r="AK20" s="96"/>
+      <c r="AL20" s="96"/>
+      <c r="AM20" s="96"/>
+      <c r="AN20" s="97"/>
+    </row>
+    <row r="21" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A21" s="98" t="s">
         <v>29</v>
       </c>
@@ -2526,21 +2637,22 @@
       <c r="AB21" s="60"/>
       <c r="AC21" s="60"/>
       <c r="AD21" s="60"/>
-      <c r="AE21" s="61"/>
-    </row>
-    <row r="22" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AE21" s="60"/>
+      <c r="AN21" s="52"/>
+    </row>
+    <row r="22" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A22" s="92" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B22" s="69">
         <v>5</v>
       </c>
       <c r="C22" s="69">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D22" s="51"/>
       <c r="E22" s="103"/>
-      <c r="F22" s="94"/>
+      <c r="F22" s="59"/>
       <c r="G22" s="59"/>
       <c r="H22" s="51"/>
       <c r="I22" s="51"/>
@@ -2565,22 +2677,23 @@
       <c r="AB22" s="51"/>
       <c r="AC22" s="51"/>
       <c r="AD22" s="51"/>
-      <c r="AE22" s="52"/>
-    </row>
-    <row r="23" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AE22" s="51"/>
+      <c r="AN22" s="52"/>
+    </row>
+    <row r="23" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A23" s="92" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B23" s="69">
         <v>2</v>
       </c>
       <c r="C23" s="69">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D23" s="51"/>
       <c r="E23" s="51"/>
-      <c r="F23" s="51"/>
-      <c r="G23" s="105"/>
+      <c r="F23" s="93"/>
+      <c r="G23" s="51"/>
       <c r="H23" s="51"/>
       <c r="I23" s="51"/>
       <c r="J23" s="51"/>
@@ -2604,24 +2717,24 @@
       <c r="AB23" s="51"/>
       <c r="AC23" s="51"/>
       <c r="AD23" s="51"/>
-      <c r="AE23" s="52"/>
-    </row>
-    <row r="24" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AE23" s="51"/>
+      <c r="AN23" s="52"/>
+    </row>
+    <row r="24" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A24" s="92" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B24" s="69">
         <v>3</v>
       </c>
       <c r="C24" s="69">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D24" s="51"/>
       <c r="E24" s="51"/>
       <c r="F24" s="51"/>
-      <c r="G24" s="51"/>
-      <c r="H24" s="93"/>
-      <c r="I24" s="51"/>
+      <c r="G24" s="93"/>
+      <c r="H24" s="43"/>
       <c r="J24" s="51"/>
       <c r="K24" s="51"/>
       <c r="L24" s="51"/>
@@ -2643,11 +2756,12 @@
       <c r="AB24" s="51"/>
       <c r="AC24" s="51"/>
       <c r="AD24" s="51"/>
-      <c r="AE24" s="52"/>
-    </row>
-    <row r="25" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AE24" s="51"/>
+      <c r="AN24" s="52"/>
+    </row>
+    <row r="25" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A25" s="92" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B25" s="69">
         <v>2</v>
@@ -2659,8 +2773,8 @@
       <c r="E25" s="51"/>
       <c r="F25" s="51"/>
       <c r="G25" s="51"/>
-      <c r="H25" s="51"/>
-      <c r="I25" s="93"/>
+      <c r="H25" s="93"/>
+      <c r="I25" s="43"/>
       <c r="J25" s="51"/>
       <c r="K25" s="51"/>
       <c r="L25" s="51"/>
@@ -2682,29 +2796,30 @@
       <c r="AB25" s="51"/>
       <c r="AC25" s="51"/>
       <c r="AD25" s="51"/>
-      <c r="AE25" s="52"/>
-    </row>
-    <row r="26" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AE25" s="51"/>
+      <c r="AN25" s="52"/>
+    </row>
+    <row r="26" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A26" s="92" t="s">
-        <v>67</v>
+        <v>86</v>
       </c>
       <c r="B26" s="69">
         <v>15</v>
       </c>
       <c r="C26" s="69">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D26" s="51"/>
       <c r="E26" s="51"/>
       <c r="F26" s="51"/>
       <c r="G26" s="51"/>
       <c r="H26" s="51"/>
-      <c r="I26" s="51"/>
+      <c r="I26" s="93"/>
       <c r="J26" s="93"/>
       <c r="K26" s="93"/>
-      <c r="L26" s="94"/>
-      <c r="M26" s="94"/>
-      <c r="N26" s="94"/>
+      <c r="L26" s="93"/>
+      <c r="M26" s="51"/>
+      <c r="N26" s="51"/>
       <c r="O26" s="51"/>
       <c r="P26" s="51"/>
       <c r="Q26" s="51"/>
@@ -2721,9 +2836,10 @@
       <c r="AB26" s="51"/>
       <c r="AC26" s="51"/>
       <c r="AD26" s="51"/>
-      <c r="AE26" s="52"/>
-    </row>
-    <row r="27" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AE26" s="51"/>
+      <c r="AN26" s="52"/>
+    </row>
+    <row r="27" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A27" s="92" t="s">
         <v>0</v>
       </c>
@@ -2742,9 +2858,9 @@
       <c r="J27" s="51"/>
       <c r="K27" s="59"/>
       <c r="L27" s="51"/>
-      <c r="M27" s="51"/>
+      <c r="M27" s="93"/>
       <c r="N27" s="51"/>
-      <c r="O27" s="93"/>
+      <c r="O27" s="51"/>
       <c r="P27" s="51"/>
       <c r="Q27" s="51"/>
       <c r="R27" s="51"/>
@@ -2760,9 +2876,10 @@
       <c r="AB27" s="51"/>
       <c r="AC27" s="51"/>
       <c r="AD27" s="51"/>
-      <c r="AE27" s="52"/>
-    </row>
-    <row r="28" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AE27" s="51"/>
+      <c r="AN27" s="52"/>
+    </row>
+    <row r="28" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="72" t="s">
         <v>1</v>
       </c>
@@ -2772,7 +2889,7 @@
       </c>
       <c r="C28" s="95">
         <f>SUM(C22:C27)</f>
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="D28" s="96"/>
       <c r="E28" s="96"/>
@@ -2801,9 +2918,18 @@
       <c r="AB28" s="96"/>
       <c r="AC28" s="96"/>
       <c r="AD28" s="96"/>
-      <c r="AE28" s="97"/>
-    </row>
-    <row r="29" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AE28" s="96"/>
+      <c r="AF28" s="96"/>
+      <c r="AG28" s="96"/>
+      <c r="AH28" s="96"/>
+      <c r="AI28" s="96"/>
+      <c r="AJ28" s="96"/>
+      <c r="AK28" s="96"/>
+      <c r="AL28" s="96"/>
+      <c r="AM28" s="96"/>
+      <c r="AN28" s="97"/>
+    </row>
+    <row r="29" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A29" s="98" t="s">
         <v>30</v>
       </c>
@@ -2836,9 +2962,10 @@
       <c r="AB29" s="60"/>
       <c r="AC29" s="60"/>
       <c r="AD29" s="60"/>
-      <c r="AE29" s="61"/>
-    </row>
-    <row r="30" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AE29" s="60"/>
+      <c r="AN29" s="52"/>
+    </row>
+    <row r="30" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A30" s="92" t="s">
         <v>34</v>
       </c>
@@ -2846,13 +2973,13 @@
         <v>6</v>
       </c>
       <c r="C30" s="69">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D30" s="51"/>
       <c r="E30" s="93"/>
       <c r="F30" s="93"/>
-      <c r="G30" s="104"/>
-      <c r="H30" s="51"/>
+      <c r="G30" s="93"/>
+      <c r="H30" s="104"/>
       <c r="I30" s="51"/>
       <c r="J30" s="51"/>
       <c r="K30" s="51"/>
@@ -2875,9 +3002,10 @@
       <c r="AB30" s="51"/>
       <c r="AC30" s="51"/>
       <c r="AD30" s="51"/>
-      <c r="AE30" s="52"/>
-    </row>
-    <row r="31" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AE30" s="51"/>
+      <c r="AN30" s="52"/>
+    </row>
+    <row r="31" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A31" s="92" t="s">
         <v>44</v>
       </c>
@@ -2885,13 +3013,13 @@
         <v>4</v>
       </c>
       <c r="C31" s="69">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D31" s="51"/>
       <c r="E31" s="51"/>
       <c r="F31" s="51"/>
       <c r="G31" s="51"/>
-      <c r="H31" s="93"/>
+      <c r="H31" s="51"/>
       <c r="I31" s="93"/>
       <c r="J31" s="104"/>
       <c r="K31" s="51"/>
@@ -2914,9 +3042,10 @@
       <c r="AB31" s="51"/>
       <c r="AC31" s="51"/>
       <c r="AD31" s="51"/>
-      <c r="AE31" s="52"/>
-    </row>
-    <row r="32" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AE31" s="51"/>
+      <c r="AN31" s="52"/>
+    </row>
+    <row r="32" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A32" s="92" t="s">
         <v>50</v>
       </c>
@@ -2924,7 +3053,7 @@
         <v>2</v>
       </c>
       <c r="C32" s="69">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D32" s="51"/>
       <c r="E32" s="51"/>
@@ -2933,7 +3062,7 @@
       <c r="H32" s="51"/>
       <c r="I32" s="51"/>
       <c r="J32" s="51"/>
-      <c r="K32" s="93"/>
+      <c r="K32" s="94"/>
       <c r="L32" s="51"/>
       <c r="M32" s="51"/>
       <c r="N32" s="51"/>
@@ -2953,11 +3082,12 @@
       <c r="AB32" s="51"/>
       <c r="AC32" s="51"/>
       <c r="AD32" s="51"/>
-      <c r="AE32" s="52"/>
-    </row>
-    <row r="33" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AE32" s="51"/>
+      <c r="AN32" s="52"/>
+    </row>
+    <row r="33" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A33" s="92" t="s">
-        <v>51</v>
+        <v>84</v>
       </c>
       <c r="B33" s="69">
         <v>4</v>
@@ -2974,7 +3104,7 @@
       <c r="J33" s="51"/>
       <c r="K33" s="51"/>
       <c r="L33" s="93"/>
-      <c r="M33" s="51"/>
+      <c r="M33" s="94"/>
       <c r="N33" s="51"/>
       <c r="O33" s="51"/>
       <c r="P33" s="51"/>
@@ -2992,17 +3122,18 @@
       <c r="AB33" s="51"/>
       <c r="AC33" s="51"/>
       <c r="AD33" s="51"/>
-      <c r="AE33" s="52"/>
-    </row>
-    <row r="34" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AE33" s="51"/>
+      <c r="AN33" s="52"/>
+    </row>
+    <row r="34" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A34" s="92" t="s">
-        <v>35</v>
+        <v>85</v>
       </c>
       <c r="B34" s="69">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C34" s="69">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D34" s="51"/>
       <c r="E34" s="51"/>
@@ -3014,8 +3145,8 @@
       <c r="K34" s="51"/>
       <c r="L34" s="51"/>
       <c r="M34" s="51"/>
-      <c r="N34" s="51"/>
-      <c r="O34" s="51"/>
+      <c r="N34" s="93"/>
+      <c r="O34" s="104"/>
       <c r="P34" s="51"/>
       <c r="Q34" s="51"/>
       <c r="R34" s="51"/>
@@ -3031,17 +3162,18 @@
       <c r="AB34" s="51"/>
       <c r="AC34" s="51"/>
       <c r="AD34" s="51"/>
-      <c r="AE34" s="52"/>
-    </row>
-    <row r="35" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AE34" s="51"/>
+      <c r="AN34" s="52"/>
+    </row>
+    <row r="35" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A35" s="92" t="s">
-        <v>0</v>
+        <v>82</v>
       </c>
       <c r="B35" s="69">
+        <v>10</v>
+      </c>
+      <c r="C35" s="69">
         <v>6</v>
-      </c>
-      <c r="C35" s="69">
-        <v>3</v>
       </c>
       <c r="D35" s="51"/>
       <c r="E35" s="51"/>
@@ -3052,13 +3184,13 @@
       <c r="J35" s="51"/>
       <c r="K35" s="51"/>
       <c r="L35" s="51"/>
-      <c r="M35" s="93"/>
+      <c r="M35" s="51"/>
       <c r="N35" s="51"/>
       <c r="O35" s="51"/>
-      <c r="P35" s="51"/>
-      <c r="Q35" s="51"/>
-      <c r="R35" s="51"/>
-      <c r="S35" s="51"/>
+      <c r="P35" s="93"/>
+      <c r="Q35" s="93"/>
+      <c r="R35" s="104"/>
+      <c r="S35" s="94"/>
       <c r="T35" s="51"/>
       <c r="U35" s="51"/>
       <c r="V35" s="51"/>
@@ -3070,138 +3202,151 @@
       <c r="AB35" s="51"/>
       <c r="AC35" s="51"/>
       <c r="AD35" s="51"/>
-      <c r="AE35" s="52"/>
-    </row>
-    <row r="36" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="72" t="s">
+      <c r="AE35" s="51"/>
+      <c r="AN35" s="52"/>
+    </row>
+    <row r="36" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A36" s="92" t="s">
+        <v>0</v>
+      </c>
+      <c r="B36" s="69">
+        <v>6</v>
+      </c>
+      <c r="C36" s="69">
+        <v>4</v>
+      </c>
+      <c r="D36" s="51"/>
+      <c r="E36" s="51"/>
+      <c r="F36" s="51"/>
+      <c r="G36" s="51"/>
+      <c r="H36" s="51"/>
+      <c r="I36" s="51"/>
+      <c r="J36" s="51"/>
+      <c r="K36" s="51"/>
+      <c r="L36" s="51"/>
+      <c r="M36" s="51"/>
+      <c r="N36" s="51"/>
+      <c r="O36" s="51"/>
+      <c r="P36" s="51"/>
+      <c r="Q36" s="51"/>
+      <c r="R36" s="51"/>
+      <c r="S36" s="51"/>
+      <c r="T36" s="93"/>
+      <c r="U36" s="94"/>
+      <c r="V36" s="51"/>
+      <c r="W36" s="51"/>
+      <c r="X36" s="51"/>
+      <c r="Y36" s="51"/>
+      <c r="Z36" s="51"/>
+      <c r="AA36" s="51"/>
+      <c r="AB36" s="51"/>
+      <c r="AC36" s="51"/>
+      <c r="AD36" s="51"/>
+      <c r="AE36" s="51"/>
+      <c r="AF36" s="43"/>
+      <c r="AN36" s="52"/>
+    </row>
+    <row r="37" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="72" t="s">
         <v>1</v>
       </c>
-      <c r="B36" s="95">
-        <f>SUM(B30:B35)</f>
-        <v>22</v>
-      </c>
-      <c r="C36" s="95">
-        <f>SUM(C30:C35)</f>
-        <v>20</v>
-      </c>
-      <c r="D36" s="96"/>
-      <c r="E36" s="96"/>
-      <c r="F36" s="96"/>
-      <c r="G36" s="96"/>
-      <c r="H36" s="96"/>
-      <c r="I36" s="96"/>
-      <c r="J36" s="96"/>
-      <c r="K36" s="96"/>
-      <c r="L36" s="96"/>
-      <c r="M36" s="96"/>
-      <c r="N36" s="96"/>
-      <c r="O36" s="96"/>
-      <c r="P36" s="96"/>
-      <c r="Q36" s="96"/>
-      <c r="R36" s="96"/>
-      <c r="S36" s="96"/>
-      <c r="T36" s="96"/>
-      <c r="U36" s="96"/>
-      <c r="V36" s="96"/>
-      <c r="W36" s="96"/>
-      <c r="X36" s="96"/>
-      <c r="Y36" s="96"/>
-      <c r="Z36" s="96"/>
-      <c r="AA36" s="96"/>
-      <c r="AB36" s="96"/>
-      <c r="AC36" s="96"/>
-      <c r="AD36" s="96"/>
-      <c r="AE36" s="97"/>
-    </row>
-    <row r="37" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A37" s="98" t="s">
+      <c r="B37" s="95">
+        <f>SUM(B30:B36)</f>
+        <v>35</v>
+      </c>
+      <c r="C37" s="95">
+        <f>SUM(C30:C36)</f>
+        <v>29</v>
+      </c>
+      <c r="D37" s="96"/>
+      <c r="E37" s="96"/>
+      <c r="F37" s="96"/>
+      <c r="G37" s="96"/>
+      <c r="H37" s="96"/>
+      <c r="I37" s="96"/>
+      <c r="J37" s="96"/>
+      <c r="K37" s="96"/>
+      <c r="L37" s="96"/>
+      <c r="M37" s="96"/>
+      <c r="N37" s="96"/>
+      <c r="O37" s="96"/>
+      <c r="P37" s="96"/>
+      <c r="Q37" s="96"/>
+      <c r="R37" s="96"/>
+      <c r="S37" s="96"/>
+      <c r="T37" s="96"/>
+      <c r="U37" s="96"/>
+      <c r="V37" s="96"/>
+      <c r="W37" s="96"/>
+      <c r="X37" s="96"/>
+      <c r="Y37" s="96"/>
+      <c r="Z37" s="96"/>
+      <c r="AA37" s="96"/>
+      <c r="AB37" s="96"/>
+      <c r="AC37" s="96"/>
+      <c r="AD37" s="96"/>
+      <c r="AE37" s="96"/>
+      <c r="AF37" s="96"/>
+      <c r="AG37" s="96"/>
+      <c r="AH37" s="96"/>
+      <c r="AI37" s="96"/>
+      <c r="AJ37" s="96"/>
+      <c r="AK37" s="96"/>
+      <c r="AL37" s="96"/>
+      <c r="AM37" s="96"/>
+      <c r="AN37" s="97"/>
+    </row>
+    <row r="38" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A38" s="98" t="s">
         <v>31</v>
       </c>
-      <c r="B37" s="88"/>
-      <c r="C37" s="88"/>
-      <c r="D37" s="60"/>
-      <c r="E37" s="60"/>
-      <c r="F37" s="60"/>
-      <c r="G37" s="60"/>
-      <c r="H37" s="60"/>
-      <c r="I37" s="60"/>
-      <c r="J37" s="60"/>
-      <c r="K37" s="60"/>
-      <c r="L37" s="60"/>
-      <c r="M37" s="60"/>
-      <c r="N37" s="60"/>
-      <c r="O37" s="60"/>
-      <c r="P37" s="60"/>
-      <c r="Q37" s="60"/>
-      <c r="R37" s="60"/>
-      <c r="S37" s="60"/>
-      <c r="T37" s="60"/>
-      <c r="U37" s="60"/>
-      <c r="V37" s="60"/>
-      <c r="W37" s="60"/>
-      <c r="X37" s="60"/>
-      <c r="Y37" s="60"/>
-      <c r="Z37" s="60"/>
-      <c r="AA37" s="60"/>
-      <c r="AB37" s="60"/>
-      <c r="AC37" s="60"/>
-      <c r="AD37" s="60"/>
-      <c r="AE37" s="61"/>
-    </row>
-    <row r="38" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A38" s="92" t="s">
+      <c r="B38" s="88"/>
+      <c r="C38" s="88"/>
+      <c r="D38" s="60"/>
+      <c r="E38" s="60"/>
+      <c r="F38" s="60"/>
+      <c r="G38" s="60"/>
+      <c r="H38" s="60"/>
+      <c r="I38" s="60"/>
+      <c r="J38" s="60"/>
+      <c r="K38" s="60"/>
+      <c r="L38" s="60"/>
+      <c r="M38" s="60"/>
+      <c r="N38" s="60"/>
+      <c r="O38" s="60"/>
+      <c r="P38" s="60"/>
+      <c r="Q38" s="60"/>
+      <c r="R38" s="60"/>
+      <c r="S38" s="60"/>
+      <c r="T38" s="60"/>
+      <c r="U38" s="60"/>
+      <c r="V38" s="60"/>
+      <c r="W38" s="60"/>
+      <c r="X38" s="60"/>
+      <c r="Y38" s="60"/>
+      <c r="Z38" s="60"/>
+      <c r="AA38" s="60"/>
+      <c r="AB38" s="60"/>
+      <c r="AC38" s="60"/>
+      <c r="AD38" s="60"/>
+      <c r="AE38" s="60"/>
+      <c r="AN38" s="52"/>
+    </row>
+    <row r="39" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A39" s="92" t="s">
         <v>46</v>
       </c>
-      <c r="B38" s="69">
+      <c r="B39" s="69">
         <v>1</v>
       </c>
-      <c r="C38" s="69">
-        <v>4</v>
-      </c>
-      <c r="D38" s="51"/>
-      <c r="E38" s="93"/>
-      <c r="F38" s="51"/>
-      <c r="G38" s="51"/>
-      <c r="H38" s="51"/>
-      <c r="I38" s="51"/>
-      <c r="J38" s="51"/>
-      <c r="K38" s="51"/>
-      <c r="L38" s="51"/>
-      <c r="M38" s="51"/>
-      <c r="N38" s="51"/>
-      <c r="O38" s="51"/>
-      <c r="P38" s="51"/>
-      <c r="Q38" s="51"/>
-      <c r="R38" s="51"/>
-      <c r="S38" s="51"/>
-      <c r="T38" s="51"/>
-      <c r="U38" s="51"/>
-      <c r="V38" s="51"/>
-      <c r="W38" s="51"/>
-      <c r="X38" s="51"/>
-      <c r="Y38" s="51"/>
-      <c r="Z38" s="51"/>
-      <c r="AA38" s="51"/>
-      <c r="AB38" s="51"/>
-      <c r="AC38" s="51"/>
-      <c r="AD38" s="51"/>
-      <c r="AE38" s="52"/>
-    </row>
-    <row r="39" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A39" s="92" t="s">
-        <v>45</v>
-      </c>
-      <c r="B39" s="69">
-        <v>10</v>
-      </c>
       <c r="C39" s="69">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D39" s="51"/>
-      <c r="E39" s="51"/>
-      <c r="F39" s="93"/>
-      <c r="G39" s="104"/>
-      <c r="H39" s="94"/>
+      <c r="E39" s="93"/>
+      <c r="F39" s="51"/>
+      <c r="G39" s="51"/>
+      <c r="H39" s="51"/>
       <c r="I39" s="51"/>
       <c r="J39" s="51"/>
       <c r="K39" s="51"/>
@@ -3224,24 +3369,25 @@
       <c r="AB39" s="51"/>
       <c r="AC39" s="51"/>
       <c r="AD39" s="51"/>
-      <c r="AE39" s="52"/>
-    </row>
-    <row r="40" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AE39" s="51"/>
+      <c r="AN39" s="52"/>
+    </row>
+    <row r="40" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A40" s="92" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B40" s="69">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C40" s="69">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D40" s="51"/>
       <c r="E40" s="51"/>
-      <c r="F40" s="51"/>
-      <c r="G40" s="51"/>
-      <c r="H40" s="51"/>
-      <c r="I40" s="93"/>
+      <c r="F40" s="93"/>
+      <c r="G40" s="104"/>
+      <c r="H40" s="94"/>
+      <c r="I40" s="51"/>
       <c r="J40" s="51"/>
       <c r="K40" s="51"/>
       <c r="L40" s="51"/>
@@ -3263,30 +3409,31 @@
       <c r="AB40" s="51"/>
       <c r="AC40" s="51"/>
       <c r="AD40" s="51"/>
-      <c r="AE40" s="52"/>
-    </row>
-    <row r="41" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AE40" s="51"/>
+      <c r="AN40" s="52"/>
+    </row>
+    <row r="41" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A41" s="92" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="B41" s="69">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="C41" s="69">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D41" s="51"/>
       <c r="E41" s="51"/>
       <c r="F41" s="51"/>
       <c r="G41" s="51"/>
       <c r="H41" s="51"/>
-      <c r="I41" s="51"/>
-      <c r="J41" s="51"/>
-      <c r="K41" s="51"/>
-      <c r="L41" s="51"/>
-      <c r="M41" s="51"/>
-      <c r="N41" s="51"/>
-      <c r="O41" s="51"/>
+      <c r="I41" s="93"/>
+      <c r="J41" s="93"/>
+      <c r="K41" s="94"/>
+      <c r="L41" s="94"/>
+      <c r="M41" s="94"/>
+      <c r="N41" s="94"/>
+      <c r="O41" s="94"/>
       <c r="P41" s="51"/>
       <c r="Q41" s="51"/>
       <c r="R41" s="51"/>
@@ -3302,17 +3449,18 @@
       <c r="AB41" s="51"/>
       <c r="AC41" s="51"/>
       <c r="AD41" s="51"/>
-      <c r="AE41" s="52"/>
-    </row>
-    <row r="42" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AE41" s="51"/>
+      <c r="AN41" s="52"/>
+    </row>
+    <row r="42" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A42" s="92" t="s">
-        <v>35</v>
+        <v>89</v>
       </c>
       <c r="B42" s="69">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C42" s="69">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D42" s="51"/>
       <c r="E42" s="51"/>
@@ -3326,7 +3474,7 @@
       <c r="M42" s="51"/>
       <c r="N42" s="51"/>
       <c r="O42" s="51"/>
-      <c r="P42" s="51"/>
+      <c r="P42" s="93"/>
       <c r="Q42" s="51"/>
       <c r="R42" s="51"/>
       <c r="S42" s="51"/>
@@ -3341,17 +3489,18 @@
       <c r="AB42" s="51"/>
       <c r="AC42" s="51"/>
       <c r="AD42" s="51"/>
-      <c r="AE42" s="52"/>
-    </row>
-    <row r="43" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AE42" s="51"/>
+      <c r="AN42" s="52"/>
+    </row>
+    <row r="43" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A43" s="92" t="s">
+        <v>35</v>
+      </c>
+      <c r="B43" s="69">
         <v>0</v>
       </c>
-      <c r="B43" s="69">
-        <v>15</v>
-      </c>
       <c r="C43" s="69">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D43" s="51"/>
       <c r="E43" s="51"/>
@@ -3359,7 +3508,7 @@
       <c r="G43" s="51"/>
       <c r="H43" s="51"/>
       <c r="I43" s="51"/>
-      <c r="J43" s="93"/>
+      <c r="J43" s="51"/>
       <c r="K43" s="51"/>
       <c r="L43" s="51"/>
       <c r="M43" s="51"/>
@@ -3380,137 +3529,149 @@
       <c r="AB43" s="51"/>
       <c r="AC43" s="51"/>
       <c r="AD43" s="51"/>
-      <c r="AE43" s="52"/>
-    </row>
-    <row r="44" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="72" t="s">
+      <c r="AE43" s="51"/>
+      <c r="AN43" s="52"/>
+    </row>
+    <row r="44" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A44" s="92" t="s">
+        <v>0</v>
+      </c>
+      <c r="B44" s="69">
+        <v>15</v>
+      </c>
+      <c r="C44" s="69">
+        <v>3</v>
+      </c>
+      <c r="D44" s="51"/>
+      <c r="E44" s="51"/>
+      <c r="F44" s="51"/>
+      <c r="G44" s="51"/>
+      <c r="H44" s="51"/>
+      <c r="I44" s="51"/>
+      <c r="J44" s="51"/>
+      <c r="K44" s="51"/>
+      <c r="L44" s="51"/>
+      <c r="M44" s="51"/>
+      <c r="N44" s="51"/>
+      <c r="O44" s="51"/>
+      <c r="P44" s="51"/>
+      <c r="Q44" s="93"/>
+      <c r="R44" s="51"/>
+      <c r="S44" s="51"/>
+      <c r="T44" s="51"/>
+      <c r="U44" s="51"/>
+      <c r="V44" s="51"/>
+      <c r="W44" s="51"/>
+      <c r="X44" s="51"/>
+      <c r="Y44" s="51"/>
+      <c r="Z44" s="51"/>
+      <c r="AA44" s="51"/>
+      <c r="AB44" s="51"/>
+      <c r="AC44" s="51"/>
+      <c r="AD44" s="51"/>
+      <c r="AE44" s="51"/>
+      <c r="AN44" s="52"/>
+    </row>
+    <row r="45" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="72" t="s">
         <v>1</v>
       </c>
-      <c r="B44" s="95">
-        <f>SUM(B38:B43)</f>
-        <v>46</v>
-      </c>
-      <c r="C44" s="95">
-        <f>SUM(C38:C43)</f>
-        <v>12</v>
-      </c>
-      <c r="D44" s="96"/>
-      <c r="E44" s="96"/>
-      <c r="F44" s="96"/>
-      <c r="G44" s="96"/>
-      <c r="H44" s="96"/>
-      <c r="I44" s="96"/>
-      <c r="J44" s="96"/>
-      <c r="K44" s="96"/>
-      <c r="L44" s="96"/>
-      <c r="M44" s="96"/>
-      <c r="N44" s="96"/>
-      <c r="O44" s="96"/>
-      <c r="P44" s="96"/>
-      <c r="Q44" s="96"/>
-      <c r="R44" s="96"/>
-      <c r="S44" s="96"/>
-      <c r="T44" s="96"/>
-      <c r="U44" s="96"/>
-      <c r="V44" s="96"/>
-      <c r="W44" s="96"/>
-      <c r="X44" s="96"/>
-      <c r="Y44" s="96"/>
-      <c r="Z44" s="96"/>
-      <c r="AA44" s="96"/>
-      <c r="AB44" s="96"/>
-      <c r="AC44" s="96"/>
-      <c r="AD44" s="96"/>
-      <c r="AE44" s="97"/>
-    </row>
-    <row r="45" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A45" s="98" t="s">
+      <c r="B45" s="95">
+        <f>SUM(B39:B44)</f>
+        <v>49</v>
+      </c>
+      <c r="C45" s="95">
+        <f>SUM(C39:C44)</f>
+        <v>17</v>
+      </c>
+      <c r="D45" s="96"/>
+      <c r="E45" s="96"/>
+      <c r="F45" s="96"/>
+      <c r="G45" s="96"/>
+      <c r="H45" s="96"/>
+      <c r="I45" s="96"/>
+      <c r="J45" s="96"/>
+      <c r="K45" s="96"/>
+      <c r="L45" s="96"/>
+      <c r="M45" s="96"/>
+      <c r="N45" s="96"/>
+      <c r="O45" s="96"/>
+      <c r="P45" s="96"/>
+      <c r="Q45" s="96"/>
+      <c r="R45" s="96"/>
+      <c r="S45" s="96"/>
+      <c r="T45" s="96"/>
+      <c r="U45" s="96"/>
+      <c r="V45" s="96"/>
+      <c r="W45" s="96"/>
+      <c r="X45" s="96"/>
+      <c r="Y45" s="96"/>
+      <c r="Z45" s="96"/>
+      <c r="AA45" s="96"/>
+      <c r="AB45" s="96"/>
+      <c r="AC45" s="96"/>
+      <c r="AD45" s="96"/>
+      <c r="AE45" s="96"/>
+      <c r="AF45" s="96"/>
+      <c r="AG45" s="96"/>
+      <c r="AH45" s="96"/>
+      <c r="AI45" s="96"/>
+      <c r="AJ45" s="96"/>
+      <c r="AK45" s="96"/>
+      <c r="AL45" s="96"/>
+      <c r="AM45" s="96"/>
+      <c r="AN45" s="97"/>
+    </row>
+    <row r="46" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A46" s="98" t="s">
         <v>32</v>
       </c>
-      <c r="B45" s="88"/>
-      <c r="C45" s="88"/>
-      <c r="D45" s="60"/>
-      <c r="E45" s="60"/>
-      <c r="F45" s="60"/>
-      <c r="G45" s="60"/>
-      <c r="H45" s="60"/>
-      <c r="I45" s="60"/>
-      <c r="J45" s="60"/>
-      <c r="K45" s="60"/>
-      <c r="L45" s="60"/>
-      <c r="M45" s="60"/>
-      <c r="N45" s="60"/>
-      <c r="O45" s="60"/>
-      <c r="P45" s="60"/>
-      <c r="Q45" s="60"/>
-      <c r="R45" s="60"/>
-      <c r="S45" s="60"/>
-      <c r="T45" s="60"/>
-      <c r="U45" s="60"/>
-      <c r="V45" s="60"/>
-      <c r="W45" s="60"/>
-      <c r="X45" s="60"/>
-      <c r="Y45" s="60"/>
-      <c r="Z45" s="60"/>
-      <c r="AA45" s="60"/>
-      <c r="AB45" s="60"/>
-      <c r="AC45" s="60"/>
-      <c r="AD45" s="60"/>
-      <c r="AE45" s="61"/>
-    </row>
-    <row r="46" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A46" s="92" t="s">
+      <c r="B46" s="88"/>
+      <c r="C46" s="88"/>
+      <c r="D46" s="60"/>
+      <c r="E46" s="60"/>
+      <c r="F46" s="60"/>
+      <c r="G46" s="60"/>
+      <c r="H46" s="60"/>
+      <c r="I46" s="60"/>
+      <c r="J46" s="60"/>
+      <c r="K46" s="60"/>
+      <c r="L46" s="60"/>
+      <c r="M46" s="60"/>
+      <c r="N46" s="60"/>
+      <c r="O46" s="60"/>
+      <c r="P46" s="60"/>
+      <c r="Q46" s="60"/>
+      <c r="R46" s="60"/>
+      <c r="S46" s="60"/>
+      <c r="T46" s="60"/>
+      <c r="U46" s="60"/>
+      <c r="V46" s="60"/>
+      <c r="W46" s="60"/>
+      <c r="X46" s="60"/>
+      <c r="Y46" s="60"/>
+      <c r="Z46" s="60"/>
+      <c r="AA46" s="60"/>
+      <c r="AB46" s="60"/>
+      <c r="AC46" s="60"/>
+      <c r="AD46" s="60"/>
+      <c r="AE46" s="60"/>
+      <c r="AN46" s="52"/>
+    </row>
+    <row r="47" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A47" s="92" t="s">
         <v>41</v>
       </c>
-      <c r="B46" s="69">
+      <c r="B47" s="69">
         <v>2</v>
-      </c>
-      <c r="C46" s="69">
-        <v>1</v>
-      </c>
-      <c r="D46" s="51"/>
-      <c r="E46" s="93"/>
-      <c r="F46" s="51"/>
-      <c r="G46" s="51"/>
-      <c r="H46" s="51"/>
-      <c r="I46" s="51"/>
-      <c r="J46" s="51"/>
-      <c r="K46" s="51"/>
-      <c r="L46" s="51"/>
-      <c r="M46" s="51"/>
-      <c r="N46" s="51"/>
-      <c r="O46" s="51"/>
-      <c r="P46" s="51"/>
-      <c r="Q46" s="51"/>
-      <c r="R46" s="51"/>
-      <c r="S46" s="51"/>
-      <c r="T46" s="51"/>
-      <c r="U46" s="51"/>
-      <c r="V46" s="51"/>
-      <c r="W46" s="51"/>
-      <c r="X46" s="51"/>
-      <c r="Y46" s="51"/>
-      <c r="Z46" s="51"/>
-      <c r="AA46" s="51"/>
-      <c r="AB46" s="51"/>
-      <c r="AC46" s="51"/>
-      <c r="AD46" s="51"/>
-      <c r="AE46" s="52"/>
-    </row>
-    <row r="47" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A47" s="92" t="s">
-        <v>33</v>
-      </c>
-      <c r="B47" s="69">
-        <v>5</v>
       </c>
       <c r="C47" s="69">
         <v>1</v>
       </c>
       <c r="D47" s="51"/>
-      <c r="E47" s="51"/>
-      <c r="F47" s="93"/>
-      <c r="G47" s="104"/>
+      <c r="E47" s="93"/>
+      <c r="F47" s="51"/>
+      <c r="G47" s="51"/>
       <c r="H47" s="51"/>
       <c r="I47" s="51"/>
       <c r="J47" s="51"/>
@@ -3534,23 +3695,24 @@
       <c r="AB47" s="51"/>
       <c r="AC47" s="51"/>
       <c r="AD47" s="51"/>
-      <c r="AE47" s="52"/>
-    </row>
-    <row r="48" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AE47" s="51"/>
+      <c r="AN47" s="52"/>
+    </row>
+    <row r="48" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A48" s="92" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B48" s="69">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C48" s="69">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D48" s="51"/>
       <c r="E48" s="51"/>
-      <c r="F48" s="51"/>
-      <c r="G48" s="51"/>
-      <c r="H48" s="51"/>
+      <c r="F48" s="93"/>
+      <c r="G48" s="104"/>
+      <c r="H48" s="94"/>
       <c r="I48" s="51"/>
       <c r="J48" s="51"/>
       <c r="K48" s="51"/>
@@ -3573,9 +3735,10 @@
       <c r="AB48" s="51"/>
       <c r="AC48" s="51"/>
       <c r="AD48" s="51"/>
-      <c r="AE48" s="52"/>
-    </row>
-    <row r="49" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AE48" s="51"/>
+      <c r="AN48" s="52"/>
+    </row>
+    <row r="49" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A49" s="92" t="s">
         <v>35</v>
       </c>
@@ -3612,9 +3775,10 @@
       <c r="AB49" s="51"/>
       <c r="AC49" s="51"/>
       <c r="AD49" s="51"/>
-      <c r="AE49" s="52"/>
-    </row>
-    <row r="50" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AE49" s="51"/>
+      <c r="AN49" s="52"/>
+    </row>
+    <row r="50" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A50" s="92" t="s">
         <v>35</v>
       </c>
@@ -3651,24 +3815,25 @@
       <c r="AB50" s="51"/>
       <c r="AC50" s="51"/>
       <c r="AD50" s="51"/>
-      <c r="AE50" s="52"/>
-    </row>
-    <row r="51" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AE50" s="51"/>
+      <c r="AN50" s="52"/>
+    </row>
+    <row r="51" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A51" s="92" t="s">
+        <v>35</v>
+      </c>
+      <c r="B51" s="69">
         <v>0</v>
       </c>
-      <c r="B51" s="69">
-        <v>5</v>
-      </c>
       <c r="C51" s="69">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D51" s="51"/>
       <c r="E51" s="51"/>
       <c r="F51" s="51"/>
       <c r="G51" s="51"/>
-      <c r="H51" s="93"/>
-      <c r="I51" s="94"/>
+      <c r="H51" s="51"/>
+      <c r="I51" s="51"/>
       <c r="J51" s="51"/>
       <c r="K51" s="51"/>
       <c r="L51" s="51"/>
@@ -3690,99 +3855,110 @@
       <c r="AB51" s="51"/>
       <c r="AC51" s="51"/>
       <c r="AD51" s="51"/>
-      <c r="AE51" s="52"/>
-    </row>
-    <row r="52" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="72" t="s">
+      <c r="AE51" s="51"/>
+      <c r="AN51" s="52"/>
+    </row>
+    <row r="52" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A52" s="92" t="s">
+        <v>0</v>
+      </c>
+      <c r="B52" s="69">
+        <v>5</v>
+      </c>
+      <c r="C52" s="69">
+        <v>2</v>
+      </c>
+      <c r="D52" s="51"/>
+      <c r="E52" s="51"/>
+      <c r="F52" s="51"/>
+      <c r="G52" s="51"/>
+      <c r="H52" s="51"/>
+      <c r="I52" s="93"/>
+      <c r="J52" s="51"/>
+      <c r="K52" s="51"/>
+      <c r="L52" s="51"/>
+      <c r="M52" s="51"/>
+      <c r="N52" s="51"/>
+      <c r="O52" s="51"/>
+      <c r="P52" s="51"/>
+      <c r="Q52" s="51"/>
+      <c r="R52" s="51"/>
+      <c r="S52" s="51"/>
+      <c r="T52" s="51"/>
+      <c r="U52" s="51"/>
+      <c r="V52" s="51"/>
+      <c r="W52" s="51"/>
+      <c r="X52" s="51"/>
+      <c r="Y52" s="51"/>
+      <c r="Z52" s="51"/>
+      <c r="AA52" s="51"/>
+      <c r="AB52" s="51"/>
+      <c r="AC52" s="51"/>
+      <c r="AD52" s="51"/>
+      <c r="AE52" s="51"/>
+      <c r="AN52" s="52"/>
+    </row>
+    <row r="53" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="72" t="s">
         <v>1</v>
       </c>
-      <c r="B52" s="95">
-        <f>SUM(B46:B51)</f>
+      <c r="B53" s="95">
+        <f>SUM(B47:B52)</f>
         <v>12</v>
       </c>
-      <c r="C52" s="95">
-        <f>SUM(C46:C51)</f>
+      <c r="C53" s="95">
+        <f>SUM(C47:C52)</f>
         <v>4</v>
       </c>
-      <c r="D52" s="96"/>
-      <c r="E52" s="96"/>
-      <c r="F52" s="96"/>
-      <c r="G52" s="96"/>
-      <c r="H52" s="96"/>
-      <c r="I52" s="96"/>
-      <c r="J52" s="96"/>
-      <c r="K52" s="96"/>
-      <c r="L52" s="96"/>
-      <c r="M52" s="96"/>
-      <c r="N52" s="96"/>
-      <c r="O52" s="96"/>
-      <c r="P52" s="96"/>
-      <c r="Q52" s="96"/>
-      <c r="R52" s="96"/>
-      <c r="S52" s="96"/>
-      <c r="T52" s="96"/>
-      <c r="U52" s="96"/>
-      <c r="V52" s="96"/>
-      <c r="W52" s="96"/>
-      <c r="X52" s="96"/>
-      <c r="Y52" s="96"/>
-      <c r="Z52" s="96"/>
-      <c r="AA52" s="96"/>
-      <c r="AB52" s="96"/>
-      <c r="AC52" s="96"/>
-      <c r="AD52" s="96"/>
-      <c r="AE52" s="97"/>
-    </row>
-    <row r="53" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="86" t="s">
+      <c r="D53" s="96"/>
+      <c r="E53" s="96"/>
+      <c r="F53" s="96"/>
+      <c r="G53" s="96"/>
+      <c r="H53" s="96"/>
+      <c r="I53" s="96"/>
+      <c r="J53" s="96"/>
+      <c r="K53" s="96"/>
+      <c r="L53" s="96"/>
+      <c r="M53" s="96"/>
+      <c r="N53" s="96"/>
+      <c r="O53" s="96"/>
+      <c r="P53" s="96"/>
+      <c r="Q53" s="96"/>
+      <c r="R53" s="96"/>
+      <c r="S53" s="96"/>
+      <c r="T53" s="96"/>
+      <c r="U53" s="96"/>
+      <c r="V53" s="96"/>
+      <c r="W53" s="96"/>
+      <c r="X53" s="96"/>
+      <c r="Y53" s="96"/>
+      <c r="Z53" s="96"/>
+      <c r="AA53" s="96"/>
+      <c r="AB53" s="96"/>
+      <c r="AC53" s="96"/>
+      <c r="AD53" s="96"/>
+      <c r="AE53" s="96"/>
+      <c r="AF53" s="96"/>
+      <c r="AG53" s="96"/>
+      <c r="AH53" s="96"/>
+      <c r="AI53" s="96"/>
+      <c r="AJ53" s="96"/>
+      <c r="AK53" s="96"/>
+      <c r="AL53" s="96"/>
+      <c r="AM53" s="96"/>
+      <c r="AN53" s="97"/>
+    </row>
+    <row r="54" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="86" t="s">
         <v>5</v>
       </c>
-      <c r="B53" s="86">
-        <f>SUM(B10,B20,B52,B28,B36,B44)</f>
-        <v>220</v>
-      </c>
-      <c r="C53" s="86">
-        <f>SUM(C26,C36,C44,C52,C10,C20)</f>
-        <v>104</v>
-      </c>
-      <c r="D53" s="43"/>
-      <c r="E53" s="43"/>
-      <c r="F53" s="43"/>
-      <c r="G53" s="43"/>
-      <c r="H53" s="43"/>
-      <c r="I53" s="43"/>
-      <c r="J53" s="43"/>
-      <c r="K53" s="43"/>
-      <c r="L53" s="43"/>
-      <c r="M53" s="43"/>
-      <c r="N53" s="43"/>
-      <c r="O53" s="43"/>
-      <c r="P53" s="43"/>
-      <c r="Q53" s="43"/>
-      <c r="R53" s="43"/>
-      <c r="S53" s="43"/>
-      <c r="T53" s="43"/>
-      <c r="U53" s="43"/>
-      <c r="V53" s="43"/>
-      <c r="W53" s="43"/>
-      <c r="X53" s="43"/>
-      <c r="Y53" s="43"/>
-      <c r="Z53" s="43"/>
-      <c r="AA53" s="43"/>
-      <c r="AB53" s="43"/>
-      <c r="AC53" s="43"/>
-    </row>
-    <row r="54" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="62" t="s">
-        <v>6</v>
-      </c>
-      <c r="B54" s="63">
-        <f>B53*100</f>
-        <v>22000</v>
-      </c>
-      <c r="C54" s="63">
-        <f>C53*100</f>
-        <v>10400</v>
+      <c r="B54" s="86">
+        <f>SUM(B11,B21,B53,B29,B37,B45)</f>
+        <v>96</v>
+      </c>
+      <c r="C54" s="86">
+        <f>SUM(C27,C37,C45,C53,C11,C21)</f>
+        <v>53</v>
       </c>
       <c r="D54" s="43"/>
       <c r="E54" s="43"/>
@@ -3810,8 +3986,21 @@
       <c r="AA54" s="43"/>
       <c r="AB54" s="43"/>
       <c r="AC54" s="43"/>
-    </row>
-    <row r="55" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AD54" s="43"/>
+      <c r="AE54" s="43"/>
+    </row>
+    <row r="55" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="62" t="s">
+        <v>6</v>
+      </c>
+      <c r="B55" s="63">
+        <f>B54*100</f>
+        <v>9600</v>
+      </c>
+      <c r="C55" s="63">
+        <f>C54*100</f>
+        <v>5300</v>
+      </c>
       <c r="D55" s="43"/>
       <c r="E55" s="43"/>
       <c r="F55" s="43"/>
@@ -3838,8 +4027,10 @@
       <c r="AA55" s="43"/>
       <c r="AB55" s="43"/>
       <c r="AC55" s="43"/>
-    </row>
-    <row r="56" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AD55" s="43"/>
+      <c r="AE55" s="43"/>
+    </row>
+    <row r="56" spans="1:40" x14ac:dyDescent="0.25">
       <c r="D56" s="43"/>
       <c r="E56" s="43"/>
       <c r="F56" s="43"/>
@@ -3867,7 +4058,7 @@
       <c r="AB56" s="43"/>
       <c r="AC56" s="43"/>
     </row>
-    <row r="57" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:40" x14ac:dyDescent="0.25">
       <c r="D57" s="43"/>
       <c r="E57" s="43"/>
       <c r="F57" s="43"/>
@@ -3895,7 +4086,7 @@
       <c r="AB57" s="43"/>
       <c r="AC57" s="43"/>
     </row>
-    <row r="58" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:40" x14ac:dyDescent="0.25">
       <c r="D58" s="43"/>
       <c r="E58" s="43"/>
       <c r="F58" s="43"/>
@@ -3923,7 +4114,7 @@
       <c r="AB58" s="43"/>
       <c r="AC58" s="43"/>
     </row>
-    <row r="59" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:40" x14ac:dyDescent="0.25">
       <c r="D59" s="43"/>
       <c r="E59" s="43"/>
       <c r="F59" s="43"/>
@@ -3951,7 +4142,7 @@
       <c r="AB59" s="43"/>
       <c r="AC59" s="43"/>
     </row>
-    <row r="60" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:40" x14ac:dyDescent="0.25">
       <c r="D60" s="43"/>
       <c r="E60" s="43"/>
       <c r="F60" s="43"/>
@@ -3979,7 +4170,7 @@
       <c r="AB60" s="43"/>
       <c r="AC60" s="43"/>
     </row>
-    <row r="61" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:40" x14ac:dyDescent="0.25">
       <c r="D61" s="43"/>
       <c r="E61" s="43"/>
       <c r="F61" s="43"/>
@@ -4007,7 +4198,7 @@
       <c r="AB61" s="43"/>
       <c r="AC61" s="43"/>
     </row>
-    <row r="62" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:40" x14ac:dyDescent="0.25">
       <c r="D62" s="43"/>
       <c r="E62" s="43"/>
       <c r="F62" s="43"/>
@@ -4035,7 +4226,7 @@
       <c r="AB62" s="43"/>
       <c r="AC62" s="43"/>
     </row>
-    <row r="63" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:40" x14ac:dyDescent="0.25">
       <c r="D63" s="43"/>
       <c r="E63" s="43"/>
       <c r="F63" s="43"/>
@@ -4063,7 +4254,7 @@
       <c r="AB63" s="43"/>
       <c r="AC63" s="43"/>
     </row>
-    <row r="64" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:40" x14ac:dyDescent="0.25">
       <c r="D64" s="43"/>
       <c r="E64" s="43"/>
       <c r="F64" s="43"/>
@@ -4157,7 +4348,7 @@
   <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N17" sqref="N17"/>
+      <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4179,19 +4370,19 @@
         <v>47</v>
       </c>
       <c r="E1" s="80" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F1" s="80" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G1" s="80" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="H1" s="80" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="I1" s="80" t="s">
-        <v>38</v>
+        <v>88</v>
       </c>
       <c r="J1" s="80" t="s">
         <v>38</v>
@@ -4215,19 +4406,19 @@
         <v>48</v>
       </c>
       <c r="E2" s="67" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F2" s="67" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G2" s="67" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H2" s="67" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="I2" s="67" t="s">
-        <v>39</v>
+        <v>87</v>
       </c>
       <c r="J2" s="67" t="s">
         <v>39</v>
@@ -4263,7 +4454,7 @@
         <v>2</v>
       </c>
       <c r="I3" s="66">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J3" s="66">
         <v>0</v>
@@ -4281,7 +4472,7 @@
       </c>
       <c r="B4" s="70">
         <f t="shared" ref="B4:B9" si="0">SUMIF(C4:L4,A$12,C$3:Z$3)</f>
-        <v>11.5</v>
+        <v>13.5</v>
       </c>
       <c r="C4" s="68" t="s">
         <v>12</v>
@@ -4301,7 +4492,9 @@
       <c r="H4" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="I4" s="69"/>
+      <c r="I4" s="68" t="s">
+        <v>12</v>
+      </c>
       <c r="J4" s="68"/>
       <c r="K4" s="68"/>
       <c r="L4" s="84"/>
@@ -4312,7 +4505,7 @@
       </c>
       <c r="B5" s="70">
         <f t="shared" si="0"/>
-        <v>11.5</v>
+        <v>13.5</v>
       </c>
       <c r="C5" s="68" t="s">
         <v>12</v>
@@ -4332,7 +4525,9 @@
       <c r="H5" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="I5" s="69"/>
+      <c r="I5" s="68" t="s">
+        <v>12</v>
+      </c>
       <c r="J5" s="68"/>
       <c r="K5" s="68"/>
       <c r="L5" s="84"/>
@@ -4343,7 +4538,7 @@
       </c>
       <c r="B6" s="70">
         <f t="shared" si="0"/>
-        <v>9.5</v>
+        <v>11.5</v>
       </c>
       <c r="C6" s="68" t="s">
         <v>12</v>
@@ -4361,7 +4556,9 @@
       <c r="H6" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="I6" s="69"/>
+      <c r="I6" s="68" t="s">
+        <v>12</v>
+      </c>
       <c r="J6" s="68"/>
       <c r="K6" s="68"/>
       <c r="L6" s="84"/>
@@ -4372,7 +4569,7 @@
       </c>
       <c r="B7" s="70">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C7" s="68"/>
       <c r="D7" s="68" t="s">
@@ -4390,7 +4587,9 @@
       <c r="H7" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="I7" s="69"/>
+      <c r="I7" s="68" t="s">
+        <v>12</v>
+      </c>
       <c r="J7" s="68"/>
       <c r="K7" s="68"/>
       <c r="L7" s="84"/>
@@ -4451,11 +4650,11 @@
     </row>
     <row r="10" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="62" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B10" s="64">
         <f>SUM(B4:B9)</f>
-        <v>57.5</v>
+        <v>65.5</v>
       </c>
       <c r="C10" s="64">
         <f>COUNTIF(C4:C9,"*ü*") * C3</f>
@@ -4483,7 +4682,7 @@
       </c>
       <c r="I10" s="64">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="J10" s="64">
         <f t="shared" si="1"/>
@@ -4645,7 +4844,7 @@
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="32"/>
       <c r="B4" s="31" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C4" s="51">
         <v>3</v>
@@ -4811,7 +5010,7 @@
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="32"/>
       <c r="B10" s="31" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C10" s="51">
         <v>3</v>
@@ -4950,7 +5149,7 @@
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="32"/>
       <c r="B15" s="31" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C15" s="51">
         <v>3</v>
@@ -5089,7 +5288,7 @@
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" s="32"/>
       <c r="B20" s="31" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C20" s="51">
         <v>3</v>
@@ -5228,7 +5427,7 @@
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" s="32"/>
       <c r="B25" s="31" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C25" s="51">
         <v>3</v>
@@ -5367,7 +5566,7 @@
     <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30" s="32"/>
       <c r="B30" s="31" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C30" s="51">
         <v>3</v>

</xml_diff>

<commit_message>
Actually Updated Gantt Chart
</commit_message>
<xml_diff>
--- a/Docs/Team_Gantt_Chart.xlsx
+++ b/Docs/Team_Gantt_Chart.xlsx
@@ -2,15 +2,16 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Brandon Foss\Documents\GitHub\6_Angry_Devs\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E8E496F-B19E-4B62-B2F8-5223E624319F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8274FBA-AB16-4826-B44E-4ABCE6694D82}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="12030" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="12030" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17625" xr2:uid="{12D7657A-059A-4288-9760-83C71639AA7A}"/>
   </bookViews>
   <sheets>
     <sheet name="Management Summary" sheetId="3" r:id="rId1"/>
@@ -974,6 +975,13 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="30" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -983,13 +991,6 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="30" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1304,10 +1305,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="B1:Q10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P25" sqref="P25"/>
+      <selection activeCell="G4" sqref="G4"/>
+    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="1">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1331,27 +1336,27 @@
   <sheetData>
     <row r="1" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="C2" s="106" t="s">
+      <c r="C2" s="113" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="107"/>
-      <c r="E2" s="108"/>
+      <c r="D2" s="114"/>
+      <c r="E2" s="115"/>
       <c r="F2" s="6"/>
-      <c r="G2" s="106" t="s">
+      <c r="G2" s="113" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="107"/>
-      <c r="I2" s="108"/>
-      <c r="K2" s="106" t="s">
+      <c r="H2" s="114"/>
+      <c r="I2" s="115"/>
+      <c r="K2" s="113" t="s">
         <v>7</v>
       </c>
-      <c r="L2" s="107"/>
-      <c r="M2" s="108"/>
-      <c r="O2" s="106" t="s">
+      <c r="L2" s="114"/>
+      <c r="M2" s="115"/>
+      <c r="O2" s="113" t="s">
         <v>26</v>
       </c>
-      <c r="P2" s="107"/>
-      <c r="Q2" s="108"/>
+      <c r="P2" s="114"/>
+      <c r="Q2" s="115"/>
     </row>
     <row r="3" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C3" s="7" t="s">
@@ -1397,15 +1402,15 @@
         <v>27</v>
       </c>
       <c r="C4" s="20">
-        <f>(G4+K4 +O4)</f>
+        <f t="shared" ref="C4:D9" si="0">(G4+K4 +O4)</f>
         <v>7000</v>
       </c>
       <c r="D4" s="21">
-        <f>(H4+L4 +P4)</f>
+        <f t="shared" si="0"/>
         <v>6550</v>
       </c>
       <c r="E4" s="22">
-        <f>(C4-D4)</f>
+        <f t="shared" ref="E4:E9" si="1">(C4-D4)</f>
         <v>450</v>
       </c>
       <c r="F4" s="3"/>
@@ -1418,10 +1423,10 @@
         <v>3600</v>
       </c>
       <c r="I4" s="16">
-        <f>(G4-H4)</f>
+        <f t="shared" ref="I4:I9" si="2">(G4-H4)</f>
         <v>100</v>
       </c>
-      <c r="K4" s="113">
+      <c r="K4" s="110">
         <v>2000</v>
       </c>
       <c r="L4" s="21">
@@ -1429,7 +1434,7 @@
         <v>1650</v>
       </c>
       <c r="M4" s="22">
-        <f>(K4-L4)</f>
+        <f t="shared" ref="M4:M9" si="3">(K4-L4)</f>
         <v>350</v>
       </c>
       <c r="O4" s="47">
@@ -1450,15 +1455,15 @@
         <v>28</v>
       </c>
       <c r="C5" s="14">
-        <f>(G5+K5 +O5)</f>
+        <f t="shared" si="0"/>
         <v>13200</v>
       </c>
       <c r="D5" s="15">
-        <f>(H5+L5 +P5)</f>
+        <f t="shared" si="0"/>
         <v>8750</v>
       </c>
       <c r="E5" s="16">
-        <f>(C5-D5)</f>
+        <f t="shared" si="1"/>
         <v>4450</v>
       </c>
       <c r="F5" s="3"/>
@@ -1471,10 +1476,10 @@
         <v>5900</v>
       </c>
       <c r="I5" s="16">
-        <f>(G5-H5)</f>
+        <f t="shared" si="2"/>
         <v>4100</v>
       </c>
-      <c r="K5" s="115">
+      <c r="K5" s="112">
         <v>2000</v>
       </c>
       <c r="L5" s="15">
@@ -1482,7 +1487,7 @@
         <v>1650</v>
       </c>
       <c r="M5" s="16">
-        <f>(K5-L5)</f>
+        <f t="shared" si="3"/>
         <v>350</v>
       </c>
       <c r="O5" s="44">
@@ -1503,15 +1508,15 @@
         <v>29</v>
       </c>
       <c r="C6" s="14">
-        <f>(G6+K6 +O6)</f>
+        <f t="shared" si="0"/>
         <v>6800</v>
       </c>
       <c r="D6" s="15">
-        <f>(H6+L6 +P6)</f>
+        <f t="shared" si="0"/>
         <v>4850</v>
       </c>
       <c r="E6" s="16">
-        <f>(C6-D6)</f>
+        <f t="shared" si="1"/>
         <v>1950</v>
       </c>
       <c r="F6" s="3"/>
@@ -1524,10 +1529,10 @@
         <v>2600</v>
       </c>
       <c r="I6" s="16">
-        <f>(G6-H6)</f>
+        <f t="shared" si="2"/>
         <v>1000</v>
       </c>
-      <c r="K6" s="115">
+      <c r="K6" s="112">
         <v>2000</v>
       </c>
       <c r="L6" s="15">
@@ -1535,7 +1540,7 @@
         <v>1150</v>
       </c>
       <c r="M6" s="16">
-        <f>(K6-L6)</f>
+        <f t="shared" si="3"/>
         <v>850</v>
       </c>
       <c r="N6" s="42"/>
@@ -1557,31 +1562,31 @@
         <v>30</v>
       </c>
       <c r="C7" s="45">
-        <f>(G7+K7 +O7)</f>
-        <v>3800</v>
+        <f t="shared" si="0"/>
+        <v>6700</v>
       </c>
       <c r="D7" s="45">
-        <f>(H7+L7 +P7)</f>
-        <v>3200</v>
+        <f t="shared" si="0"/>
+        <v>6400</v>
       </c>
       <c r="E7" s="46">
-        <f>(C7-D7)</f>
-        <v>600</v>
+        <f t="shared" si="1"/>
+        <v>300</v>
       </c>
       <c r="F7" s="3"/>
       <c r="G7" s="14">
-        <f>(Gantt!$B37)*100</f>
-        <v>600</v>
+        <f>(Gantt!$B38)*100</f>
+        <v>3500</v>
       </c>
       <c r="H7" s="15">
-        <f>(Gantt!$C37)*100</f>
-        <v>600</v>
+        <f>(Gantt!$C38)*100</f>
+        <v>3800</v>
       </c>
       <c r="I7" s="16">
-        <f>(G7-H7)</f>
-        <v>0</v>
-      </c>
-      <c r="K7" s="115">
+        <f t="shared" si="2"/>
+        <v>-300</v>
+      </c>
+      <c r="K7" s="112">
         <v>2000</v>
       </c>
       <c r="L7" s="15">
@@ -1589,7 +1594,7 @@
         <v>1500</v>
       </c>
       <c r="M7" s="16">
-        <f>(K7-L7)</f>
+        <f t="shared" si="3"/>
         <v>500</v>
       </c>
       <c r="N7" s="42"/>
@@ -1602,7 +1607,7 @@
         <v>1100</v>
       </c>
       <c r="Q7" s="57">
-        <f t="shared" ref="Q5:Q7" si="0">(O7-P7)</f>
+        <f t="shared" ref="Q7" si="4">(O7-P7)</f>
         <v>100</v>
       </c>
     </row>
@@ -1611,31 +1616,31 @@
         <v>31</v>
       </c>
       <c r="C8" s="45">
-        <f>(G8+K8 +O8)</f>
-        <v>4700</v>
+        <f t="shared" si="0"/>
+        <v>9300</v>
       </c>
       <c r="D8" s="45">
-        <f>(H8+L8 +P8)</f>
-        <v>2950</v>
+        <f t="shared" si="0"/>
+        <v>5050</v>
       </c>
       <c r="E8" s="46">
-        <f>(C8-D8)</f>
-        <v>1750</v>
+        <f t="shared" si="1"/>
+        <v>4250</v>
       </c>
       <c r="F8" s="3"/>
       <c r="G8" s="14">
-        <f>(Gantt!$B45)*100</f>
-        <v>1500</v>
+        <f>(Gantt!$B46)*100</f>
+        <v>6100</v>
       </c>
       <c r="H8" s="15">
-        <f>(Gantt!$C45)*100</f>
-        <v>800</v>
+        <f>(Gantt!$C46)*100</f>
+        <v>2900</v>
       </c>
       <c r="I8" s="16">
-        <f>(G8-H8)</f>
-        <v>700</v>
-      </c>
-      <c r="K8" s="115">
+        <f t="shared" si="2"/>
+        <v>3200</v>
+      </c>
+      <c r="K8" s="112">
         <v>2000</v>
       </c>
       <c r="L8" s="15">
@@ -1643,7 +1648,7 @@
         <v>950</v>
       </c>
       <c r="M8" s="16">
-        <f>(K8-L8)</f>
+        <f t="shared" si="3"/>
         <v>1050</v>
       </c>
       <c r="N8" s="42"/>
@@ -1665,30 +1670,30 @@
         <v>32</v>
       </c>
       <c r="C9" s="40">
-        <f>(G9+K9 +O9)</f>
-        <v>3700</v>
+        <f t="shared" si="0"/>
+        <v>5400</v>
       </c>
       <c r="D9" s="41">
-        <f>(H9+L9 +P9)</f>
-        <v>1350</v>
+        <f t="shared" si="0"/>
+        <v>2150</v>
       </c>
       <c r="E9" s="27">
-        <f>(C9-D9)</f>
-        <v>2350</v>
+        <f t="shared" si="1"/>
+        <v>3250</v>
       </c>
       <c r="G9" s="14">
-        <f>(Gantt!$B53)*100</f>
-        <v>500</v>
+        <f>(Gantt!$B54)*100</f>
+        <v>2200</v>
       </c>
       <c r="H9" s="15">
-        <f>(Gantt!$C53)*100</f>
-        <v>400</v>
+        <f>(Gantt!$C54)*100</f>
+        <v>1200</v>
       </c>
       <c r="I9" s="16">
-        <f>(G9-H9)</f>
-        <v>100</v>
-      </c>
-      <c r="K9" s="114">
+        <f t="shared" si="2"/>
+        <v>1000</v>
+      </c>
+      <c r="K9" s="111">
         <v>2000</v>
       </c>
       <c r="L9" s="15">
@@ -1696,7 +1701,7 @@
         <v>550</v>
       </c>
       <c r="M9" s="16">
-        <f>(K9-L9)</f>
+        <f t="shared" si="3"/>
         <v>1450</v>
       </c>
       <c r="O9" s="54">
@@ -1718,27 +1723,27 @@
       </c>
       <c r="C10" s="24">
         <f>SUM(C4:C9)</f>
-        <v>39200</v>
+        <v>48400</v>
       </c>
       <c r="D10" s="25">
         <f>SUM(D4:D9)</f>
-        <v>27650</v>
+        <v>33750</v>
       </c>
       <c r="E10" s="26">
         <f>SUM(E4:E9)</f>
-        <v>11550</v>
+        <v>14650</v>
       </c>
       <c r="G10" s="17">
         <f>SUM(G4:G9)</f>
-        <v>19900</v>
+        <v>29100</v>
       </c>
       <c r="H10" s="18">
         <f>SUM(H4:H9)</f>
-        <v>13900</v>
+        <v>20000</v>
       </c>
       <c r="I10" s="19">
         <f>SUM(I4:I9)</f>
-        <v>6000</v>
+        <v>9100</v>
       </c>
       <c r="K10" s="17">
         <f>SUM(K4:K9)</f>
@@ -1779,10 +1784,14 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:AZ66"/>
   <sheetViews>
-    <sheetView zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="B57" sqref="B57"/>
+    <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="S58" sqref="S58"/>
+    </sheetView>
+    <sheetView workbookViewId="1">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1922,31 +1931,31 @@
         <v>96</v>
       </c>
       <c r="AK2" s="90">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="AL2" s="90">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="AM2" s="90">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="AN2" s="90">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="AO2" s="90">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="AP2" s="90">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="AQ2" s="90">
-        <v>108</v>
+        <v>117</v>
       </c>
       <c r="AR2" s="90">
-        <v>109</v>
+        <v>120</v>
       </c>
       <c r="AS2" s="90">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="AT2" s="43"/>
       <c r="AU2" s="43"/>
@@ -1999,7 +2008,7 @@
       <c r="AP3" s="43"/>
       <c r="AQ3" s="43"/>
       <c r="AR3" s="43"/>
-      <c r="AS3" s="109"/>
+      <c r="AS3" s="106"/>
       <c r="AT3" s="43"/>
       <c r="AU3" s="43"/>
       <c r="AV3" s="43"/>
@@ -2051,7 +2060,7 @@
       <c r="AP4" s="43"/>
       <c r="AQ4" s="43"/>
       <c r="AR4" s="43"/>
-      <c r="AS4" s="110"/>
+      <c r="AS4" s="107"/>
       <c r="AT4" s="43"/>
       <c r="AU4" s="43"/>
       <c r="AV4" s="43"/>
@@ -2103,7 +2112,7 @@
       <c r="AP5" s="43"/>
       <c r="AQ5" s="43"/>
       <c r="AR5" s="43"/>
-      <c r="AS5" s="110"/>
+      <c r="AS5" s="107"/>
       <c r="AT5" s="43"/>
       <c r="AU5" s="43"/>
       <c r="AV5" s="43"/>
@@ -2155,7 +2164,7 @@
       <c r="AP6" s="43"/>
       <c r="AQ6" s="43"/>
       <c r="AR6" s="43"/>
-      <c r="AS6" s="110"/>
+      <c r="AS6" s="107"/>
       <c r="AT6" s="43"/>
       <c r="AU6" s="43"/>
       <c r="AV6" s="43"/>
@@ -2207,7 +2216,7 @@
       <c r="AP7" s="43"/>
       <c r="AQ7" s="43"/>
       <c r="AR7" s="43"/>
-      <c r="AS7" s="110"/>
+      <c r="AS7" s="107"/>
       <c r="AT7" s="43"/>
       <c r="AU7" s="43"/>
       <c r="AV7" s="43"/>
@@ -2259,7 +2268,7 @@
       <c r="AP8" s="43"/>
       <c r="AQ8" s="43"/>
       <c r="AR8" s="43"/>
-      <c r="AS8" s="110"/>
+      <c r="AS8" s="107"/>
       <c r="AT8" s="43"/>
       <c r="AU8" s="43"/>
       <c r="AV8" s="43"/>
@@ -2311,7 +2320,7 @@
       <c r="AP9" s="43"/>
       <c r="AQ9" s="43"/>
       <c r="AR9" s="43"/>
-      <c r="AS9" s="110"/>
+      <c r="AS9" s="107"/>
       <c r="AT9" s="43"/>
       <c r="AU9" s="43"/>
       <c r="AV9" s="43"/>
@@ -2373,7 +2382,7 @@
       <c r="AP10" s="96"/>
       <c r="AQ10" s="96"/>
       <c r="AR10" s="96"/>
-      <c r="AS10" s="111"/>
+      <c r="AS10" s="108"/>
       <c r="AT10" s="43"/>
       <c r="AU10" s="43"/>
       <c r="AV10" s="43"/>
@@ -2421,7 +2430,7 @@
       <c r="AP11" s="43"/>
       <c r="AQ11" s="43"/>
       <c r="AR11" s="43"/>
-      <c r="AS11" s="110"/>
+      <c r="AS11" s="107"/>
       <c r="AT11" s="43"/>
       <c r="AU11" s="43"/>
       <c r="AV11" s="43"/>
@@ -2473,7 +2482,7 @@
       <c r="AP12" s="43"/>
       <c r="AQ12" s="43"/>
       <c r="AR12" s="43"/>
-      <c r="AS12" s="110"/>
+      <c r="AS12" s="107"/>
       <c r="AT12" s="43"/>
       <c r="AU12" s="43"/>
       <c r="AV12" s="43"/>
@@ -2525,7 +2534,7 @@
       <c r="AP13" s="43"/>
       <c r="AQ13" s="43"/>
       <c r="AR13" s="43"/>
-      <c r="AS13" s="110"/>
+      <c r="AS13" s="107"/>
       <c r="AT13" s="43"/>
       <c r="AU13" s="43"/>
       <c r="AV13" s="43"/>
@@ -2577,7 +2586,7 @@
       <c r="AP14" s="43"/>
       <c r="AQ14" s="43"/>
       <c r="AR14" s="43"/>
-      <c r="AS14" s="110"/>
+      <c r="AS14" s="107"/>
       <c r="AT14" s="43"/>
       <c r="AU14" s="43"/>
       <c r="AV14" s="43"/>
@@ -2629,7 +2638,7 @@
       <c r="AP15" s="43"/>
       <c r="AQ15" s="43"/>
       <c r="AR15" s="43"/>
-      <c r="AS15" s="110"/>
+      <c r="AS15" s="107"/>
       <c r="AT15" s="43"/>
       <c r="AU15" s="43"/>
       <c r="AV15" s="43"/>
@@ -2681,7 +2690,7 @@
       <c r="AP16" s="43"/>
       <c r="AQ16" s="43"/>
       <c r="AR16" s="43"/>
-      <c r="AS16" s="110"/>
+      <c r="AS16" s="107"/>
       <c r="AT16" s="43"/>
       <c r="AU16" s="43"/>
       <c r="AV16" s="43"/>
@@ -2738,7 +2747,7 @@
       <c r="AP17" s="43"/>
       <c r="AQ17" s="43"/>
       <c r="AR17" s="43"/>
-      <c r="AS17" s="110"/>
+      <c r="AS17" s="107"/>
       <c r="AT17" s="43"/>
       <c r="AU17" s="43"/>
       <c r="AV17" s="43"/>
@@ -2793,7 +2802,7 @@
       <c r="AP18" s="43"/>
       <c r="AQ18" s="43"/>
       <c r="AR18" s="43"/>
-      <c r="AS18" s="110"/>
+      <c r="AS18" s="107"/>
       <c r="AT18" s="43"/>
       <c r="AU18" s="43"/>
       <c r="AV18" s="43"/>
@@ -2848,7 +2857,7 @@
       <c r="AP19" s="4"/>
       <c r="AQ19" s="4"/>
       <c r="AR19" s="4"/>
-      <c r="AS19" s="112"/>
+      <c r="AS19" s="109"/>
       <c r="AT19" s="43"/>
       <c r="AU19" s="43"/>
       <c r="AV19" s="43"/>
@@ -2910,7 +2919,7 @@
       <c r="AP20" s="96"/>
       <c r="AQ20" s="96"/>
       <c r="AR20" s="96"/>
-      <c r="AS20" s="111"/>
+      <c r="AS20" s="108"/>
       <c r="AT20" s="43"/>
       <c r="AU20" s="43"/>
       <c r="AV20" s="43"/>
@@ -2958,7 +2967,7 @@
       <c r="AP21" s="43"/>
       <c r="AQ21" s="43"/>
       <c r="AR21" s="43"/>
-      <c r="AS21" s="110"/>
+      <c r="AS21" s="107"/>
       <c r="AT21" s="43"/>
       <c r="AU21" s="43"/>
       <c r="AV21" s="43"/>
@@ -3010,7 +3019,7 @@
       <c r="AP22" s="43"/>
       <c r="AQ22" s="43"/>
       <c r="AR22" s="43"/>
-      <c r="AS22" s="110"/>
+      <c r="AS22" s="107"/>
       <c r="AT22" s="43"/>
       <c r="AU22" s="43"/>
       <c r="AV22" s="43"/>
@@ -3062,7 +3071,7 @@
       <c r="AP23" s="43"/>
       <c r="AQ23" s="43"/>
       <c r="AR23" s="43"/>
-      <c r="AS23" s="110"/>
+      <c r="AS23" s="107"/>
       <c r="AT23" s="43"/>
       <c r="AU23" s="43"/>
       <c r="AV23" s="43"/>
@@ -3113,7 +3122,7 @@
       <c r="AP24" s="43"/>
       <c r="AQ24" s="43"/>
       <c r="AR24" s="43"/>
-      <c r="AS24" s="110"/>
+      <c r="AS24" s="107"/>
       <c r="AT24" s="43"/>
       <c r="AU24" s="43"/>
       <c r="AV24" s="43"/>
@@ -3165,7 +3174,7 @@
       <c r="AP25" s="43"/>
       <c r="AQ25" s="43"/>
       <c r="AR25" s="43"/>
-      <c r="AS25" s="110"/>
+      <c r="AS25" s="107"/>
       <c r="AT25" s="43"/>
       <c r="AU25" s="43"/>
       <c r="AV25" s="43"/>
@@ -3217,7 +3226,7 @@
       <c r="AP26" s="43"/>
       <c r="AQ26" s="43"/>
       <c r="AR26" s="43"/>
-      <c r="AS26" s="110"/>
+      <c r="AS26" s="107"/>
       <c r="AT26" s="43"/>
       <c r="AU26" s="43"/>
       <c r="AV26" s="43"/>
@@ -3269,7 +3278,7 @@
       <c r="AP27" s="43"/>
       <c r="AQ27" s="43"/>
       <c r="AR27" s="43"/>
-      <c r="AS27" s="110"/>
+      <c r="AS27" s="107"/>
       <c r="AT27" s="43"/>
       <c r="AU27" s="43"/>
       <c r="AV27" s="43"/>
@@ -3296,7 +3305,7 @@
       <c r="AP28" s="43"/>
       <c r="AQ28" s="43"/>
       <c r="AR28" s="43"/>
-      <c r="AS28" s="110"/>
+      <c r="AS28" s="107"/>
       <c r="AT28" s="43"/>
       <c r="AU28" s="43"/>
       <c r="AV28" s="43"/>
@@ -3358,7 +3367,7 @@
       <c r="AP29" s="96"/>
       <c r="AQ29" s="96"/>
       <c r="AR29" s="96"/>
-      <c r="AS29" s="111"/>
+      <c r="AS29" s="108"/>
       <c r="AT29" s="43"/>
       <c r="AU29" s="43"/>
       <c r="AV29" s="43"/>
@@ -3406,7 +3415,7 @@
       <c r="AP30" s="43"/>
       <c r="AQ30" s="43"/>
       <c r="AR30" s="43"/>
-      <c r="AS30" s="110"/>
+      <c r="AS30" s="107"/>
       <c r="AT30" s="43"/>
       <c r="AU30" s="43"/>
       <c r="AV30" s="43"/>
@@ -3458,7 +3467,7 @@
       <c r="AP31" s="43"/>
       <c r="AQ31" s="43"/>
       <c r="AR31" s="43"/>
-      <c r="AS31" s="110"/>
+      <c r="AS31" s="107"/>
       <c r="AT31" s="43"/>
       <c r="AU31" s="43"/>
       <c r="AV31" s="43"/>
@@ -3510,7 +3519,7 @@
       <c r="AP32" s="43"/>
       <c r="AQ32" s="43"/>
       <c r="AR32" s="43"/>
-      <c r="AS32" s="110"/>
+      <c r="AS32" s="107"/>
       <c r="AT32" s="43"/>
       <c r="AU32" s="43"/>
       <c r="AV32" s="43"/>
@@ -3562,7 +3571,7 @@
       <c r="AP33" s="43"/>
       <c r="AQ33" s="43"/>
       <c r="AR33" s="43"/>
-      <c r="AS33" s="110"/>
+      <c r="AS33" s="107"/>
       <c r="AT33" s="43"/>
       <c r="AU33" s="43"/>
       <c r="AV33" s="43"/>
@@ -3614,7 +3623,7 @@
       <c r="AP34" s="43"/>
       <c r="AQ34" s="43"/>
       <c r="AR34" s="43"/>
-      <c r="AS34" s="110"/>
+      <c r="AS34" s="107"/>
       <c r="AT34" s="43"/>
       <c r="AU34" s="43"/>
       <c r="AV34" s="43"/>
@@ -3666,7 +3675,7 @@
       <c r="AP35" s="43"/>
       <c r="AQ35" s="43"/>
       <c r="AR35" s="43"/>
-      <c r="AS35" s="110"/>
+      <c r="AS35" s="107"/>
       <c r="AT35" s="43"/>
       <c r="AU35" s="43"/>
       <c r="AV35" s="43"/>
@@ -3718,7 +3727,7 @@
       <c r="AP36" s="43"/>
       <c r="AQ36" s="43"/>
       <c r="AR36" s="43"/>
-      <c r="AS36" s="110"/>
+      <c r="AS36" s="107"/>
       <c r="AT36" s="43"/>
       <c r="AU36" s="43"/>
       <c r="AV36" s="43"/>
@@ -3771,7 +3780,7 @@
       <c r="AP37" s="43"/>
       <c r="AQ37" s="43"/>
       <c r="AR37" s="43"/>
-      <c r="AS37" s="110"/>
+      <c r="AS37" s="107"/>
       <c r="AT37" s="43"/>
       <c r="AU37" s="43"/>
       <c r="AV37" s="43"/>
@@ -3833,7 +3842,7 @@
       <c r="AP38" s="96"/>
       <c r="AQ38" s="96"/>
       <c r="AR38" s="96"/>
-      <c r="AS38" s="111"/>
+      <c r="AS38" s="108"/>
       <c r="AT38" s="43"/>
       <c r="AU38" s="43"/>
       <c r="AV38" s="43"/>
@@ -3881,7 +3890,7 @@
       <c r="AP39" s="43"/>
       <c r="AQ39" s="43"/>
       <c r="AR39" s="43"/>
-      <c r="AS39" s="110"/>
+      <c r="AS39" s="107"/>
       <c r="AT39" s="43"/>
       <c r="AU39" s="43"/>
       <c r="AV39" s="43"/>
@@ -3933,7 +3942,7 @@
       <c r="AP40" s="43"/>
       <c r="AQ40" s="43"/>
       <c r="AR40" s="43"/>
-      <c r="AS40" s="110"/>
+      <c r="AS40" s="107"/>
       <c r="AT40" s="43"/>
       <c r="AU40" s="43"/>
       <c r="AV40" s="43"/>
@@ -3985,7 +3994,7 @@
       <c r="AP41" s="43"/>
       <c r="AQ41" s="43"/>
       <c r="AR41" s="43"/>
-      <c r="AS41" s="110"/>
+      <c r="AS41" s="107"/>
       <c r="AT41" s="43"/>
       <c r="AU41" s="43"/>
       <c r="AV41" s="43"/>
@@ -4037,7 +4046,7 @@
       <c r="AP42" s="43"/>
       <c r="AQ42" s="43"/>
       <c r="AR42" s="43"/>
-      <c r="AS42" s="110"/>
+      <c r="AS42" s="107"/>
       <c r="AT42" s="43"/>
       <c r="AU42" s="43"/>
       <c r="AV42" s="43"/>
@@ -4089,7 +4098,7 @@
       <c r="AP43" s="43"/>
       <c r="AQ43" s="43"/>
       <c r="AR43" s="43"/>
-      <c r="AS43" s="110"/>
+      <c r="AS43" s="107"/>
       <c r="AT43" s="43"/>
       <c r="AU43" s="43"/>
       <c r="AV43" s="43"/>
@@ -4141,7 +4150,7 @@
       <c r="AP44" s="43"/>
       <c r="AQ44" s="43"/>
       <c r="AR44" s="43"/>
-      <c r="AS44" s="110"/>
+      <c r="AS44" s="107"/>
       <c r="AT44" s="43"/>
       <c r="AU44" s="43"/>
       <c r="AV44" s="43"/>
@@ -4193,7 +4202,7 @@
       <c r="AP45" s="43"/>
       <c r="AQ45" s="43"/>
       <c r="AR45" s="43"/>
-      <c r="AS45" s="110"/>
+      <c r="AS45" s="107"/>
       <c r="AT45" s="43"/>
       <c r="AU45" s="43"/>
       <c r="AV45" s="43"/>
@@ -4255,7 +4264,7 @@
       <c r="AP46" s="96"/>
       <c r="AQ46" s="96"/>
       <c r="AR46" s="96"/>
-      <c r="AS46" s="111"/>
+      <c r="AS46" s="108"/>
       <c r="AT46" s="43"/>
       <c r="AU46" s="43"/>
       <c r="AV46" s="43"/>
@@ -4303,7 +4312,7 @@
       <c r="AP47" s="43"/>
       <c r="AQ47" s="43"/>
       <c r="AR47" s="43"/>
-      <c r="AS47" s="110"/>
+      <c r="AS47" s="107"/>
       <c r="AT47" s="43"/>
       <c r="AU47" s="43"/>
       <c r="AV47" s="43"/>
@@ -4355,7 +4364,7 @@
       <c r="AP48" s="43"/>
       <c r="AQ48" s="43"/>
       <c r="AR48" s="43"/>
-      <c r="AS48" s="110"/>
+      <c r="AS48" s="107"/>
       <c r="AT48" s="43"/>
       <c r="AU48" s="43"/>
       <c r="AV48" s="43"/>
@@ -4407,7 +4416,7 @@
       <c r="AP49" s="43"/>
       <c r="AQ49" s="43"/>
       <c r="AR49" s="43"/>
-      <c r="AS49" s="110"/>
+      <c r="AS49" s="107"/>
       <c r="AT49" s="43"/>
       <c r="AU49" s="43"/>
       <c r="AV49" s="43"/>
@@ -4459,7 +4468,7 @@
       <c r="AP50" s="43"/>
       <c r="AQ50" s="43"/>
       <c r="AR50" s="43"/>
-      <c r="AS50" s="110"/>
+      <c r="AS50" s="107"/>
       <c r="AT50" s="43"/>
       <c r="AU50" s="43"/>
       <c r="AV50" s="43"/>
@@ -4511,7 +4520,7 @@
       <c r="AP51" s="43"/>
       <c r="AQ51" s="43"/>
       <c r="AR51" s="43"/>
-      <c r="AS51" s="110"/>
+      <c r="AS51" s="107"/>
       <c r="AT51" s="43"/>
       <c r="AU51" s="43"/>
       <c r="AV51" s="43"/>
@@ -4563,7 +4572,7 @@
       <c r="AP52" s="43"/>
       <c r="AQ52" s="43"/>
       <c r="AR52" s="43"/>
-      <c r="AS52" s="110"/>
+      <c r="AS52" s="107"/>
       <c r="AT52" s="43"/>
       <c r="AU52" s="43"/>
       <c r="AV52" s="43"/>
@@ -4615,7 +4624,7 @@
       <c r="AP53" s="43"/>
       <c r="AQ53" s="43"/>
       <c r="AR53" s="43"/>
-      <c r="AS53" s="110"/>
+      <c r="AS53" s="107"/>
       <c r="AT53" s="43"/>
       <c r="AU53" s="43"/>
       <c r="AV53" s="43"/>
@@ -4677,7 +4686,7 @@
       <c r="AP54" s="96"/>
       <c r="AQ54" s="96"/>
       <c r="AR54" s="96"/>
-      <c r="AS54" s="111"/>
+      <c r="AS54" s="108"/>
       <c r="AT54" s="43"/>
       <c r="AU54" s="43"/>
       <c r="AV54" s="43"/>
@@ -5062,16 +5071,19 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H41" sqref="H41"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5386,43 +5398,43 @@
         <v>74.5</v>
       </c>
       <c r="C10" s="64">
-        <f>COUNTIF(C4:C9,"*ü*") * C3</f>
+        <f t="shared" ref="C10:L10" si="1">COUNTIF(C4:C9,"*ü*") * C3</f>
         <v>7.5</v>
       </c>
       <c r="D10" s="64">
-        <f>COUNTIF(D4:D9,"*ü*") * D3</f>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="E10" s="64">
-        <f>COUNTIF(E4:E9,"*ü*") * E3</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="F10" s="64">
-        <f>COUNTIF(F4:F9,"*ü*") * F3</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="G10" s="64">
-        <f>COUNTIF(G4:G9,"*ü*") * G3</f>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="H10" s="64">
-        <f>COUNTIF(H4:H9,"*ü*") * H3</f>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="I10" s="64">
-        <f>COUNTIF(I4:I9,"*ü*") * I3</f>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="J10" s="64">
-        <f>COUNTIF(J4:J9,"*ü*") * J3</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="K10" s="64">
-        <f>COUNTIF(K4:K9,"*ü*") * K3</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="L10" s="64">
-        <f>COUNTIF(L4:L9,"*ü*") * L3</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -5442,11 +5454,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:S34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I44" sqref="I44"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F45" sqref="F45"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>